<commit_message>
fixed bugs on the GUIs and update the ini generators
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/forearm_ini_generator iCubV2.xlsx
+++ b/app/skinGui/iniGenerators/forearm_ini_generator iCubV2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12975"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="lower" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -653,7 +653,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4434,8 +4433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4469,81 +4468,81 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="56" t="s">
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="34" t="s">
+      <c r="P2" s="33" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <f t="shared" ref="B3:B5" si="0">((ROUND($L3/10,0))-1)*4+MOD($L3,10)+((J3-1)*16)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <f>((+O3*COS($N$3)-P3*SIN($N$3)+$N$7)*$R$3)</f>
         <v>100</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <f>((O3*SIN($N$3)+P3*COS($N$3)+$N$9)*$R$4)</f>
         <v>-20</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)+$N$5)</f>
-        <v>-90</v>
+        <v>29.999719388456853</v>
       </c>
       <c r="F3" s="11">
         <v>5</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <f t="shared" ref="G3:G5" si="1">IF($R$3*$R$4=-1,1,0)</f>
         <v>1</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="40">
+      <c r="J3" s="39">
         <v>1</v>
       </c>
       <c r="K3" s="12">
@@ -4552,59 +4551,59 @@
       <c r="L3" s="13">
         <v>10</v>
       </c>
-      <c r="M3" s="14">
-        <v>0</v>
-      </c>
-      <c r="N3" s="15">
+      <c r="M3" s="6">
+        <v>-2.0943951023932001</v>
+      </c>
+      <c r="N3" s="14">
         <f>+RADIANS(N5)</f>
         <v>1.5707963267948966</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="15">
         <v>100</v>
       </c>
-      <c r="P3" s="41">
+      <c r="P3" s="40">
         <v>100</v>
       </c>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="53">
+      <c r="R3" s="52">
         <v>-1</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <f>((+O4*COS($N$3)-P4*SIN($N$3)+$N$7)*$R$3)</f>
         <v>109.23760430703399</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <f>((O4*SIN($N$3)+P4*COS($N$3)+$N$9)*$R$4)</f>
         <v>-4</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M4/3.1416*180)+$N$5)</f>
         <v>-30.000140305771573</v>
       </c>
       <c r="F4" s="11">
         <v>5</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="42">
+      <c r="J4" s="41">
         <v>1</v>
       </c>
       <c r="K4" s="10">
@@ -4619,50 +4618,50 @@
       <c r="N4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="43">
+      <c r="O4" s="42">
         <v>116</v>
       </c>
-      <c r="P4" s="44">
+      <c r="P4" s="43">
         <v>109.237604307034</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="55">
+      <c r="R4" s="54">
         <v>1</v>
       </c>
       <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <f>((+O5*COS($N$3)-P5*SIN($N$3)+$N$7)*$R$3)</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <f>((O5*SIN($N$3)+P5*COS($N$3)+$N$9)*$R$4)</f>
         <v>12</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M5/3.1416*180)+$N$5)</f>
         <v>29.999719388456853</v>
       </c>
       <c r="F5" s="11">
         <v>5</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="42">
+      <c r="J5" s="41">
         <v>1</v>
       </c>
       <c r="K5" s="10">
@@ -4677,30 +4676,30 @@
       <c r="N5" s="3">
         <v>90</v>
       </c>
-      <c r="O5" s="43">
+      <c r="O5" s="42">
         <v>132</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="43">
         <v>100</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="26"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="42">
+      <c r="J6" s="41">
         <v>1</v>
       </c>
       <c r="K6" s="10">
@@ -4712,31 +4711,31 @@
       <c r="M6" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N6" s="45" t="s">
+      <c r="N6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="43">
+      <c r="O6" s="42">
         <v>148</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="43">
         <v>109.237604307034</v>
       </c>
       <c r="S6" s="9"/>
-      <c r="T6" s="18" t="s">
+      <c r="T6" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="26"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="42">
+      <c r="J7" s="41">
         <v>1</v>
       </c>
       <c r="K7" s="10">
@@ -4751,27 +4750,27 @@
       <c r="N7" s="3">
         <v>0</v>
       </c>
-      <c r="O7" s="43">
+      <c r="O7" s="42">
         <v>148</v>
       </c>
-      <c r="P7" s="44">
+      <c r="P7" s="43">
         <v>127.712812921102</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="T7" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="26"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="42">
+      <c r="J8" s="41">
         <v>1</v>
       </c>
       <c r="K8" s="10">
@@ -4783,29 +4782,29 @@
       <c r="M8" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N8" s="45" t="s">
+      <c r="N8" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="43">
+      <c r="O8" s="42">
         <v>164</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="43">
         <v>136.95041722813599</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="26"/>
+      <c r="G9" s="25"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="42">
+      <c r="J9" s="41">
         <v>1</v>
       </c>
       <c r="K9" s="10">
@@ -4820,24 +4819,24 @@
       <c r="N9" s="3">
         <v>-120</v>
       </c>
-      <c r="O9" s="43">
+      <c r="O9" s="42">
         <v>164</v>
       </c>
-      <c r="P9" s="44">
+      <c r="P9" s="43">
         <v>155.425625842204</v>
       </c>
       <c r="T9" s="7"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="26"/>
+      <c r="G10" s="25"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="42">
+      <c r="J10" s="41">
         <v>1</v>
       </c>
       <c r="K10" s="10">
@@ -4852,42 +4851,42 @@
       <c r="N10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="43">
+      <c r="O10" s="42">
         <v>148</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <f t="shared" ref="B11:B20" si="2">((ROUND($L11/10,0))-1)*4+MOD($L11,10)+((J11-1)*16)</f>
         <v>12</v>
       </c>
-      <c r="C11" s="24">
-        <f>((+O11*COS($N$3)-P11*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C11" s="23">
+        <f t="shared" ref="C11:C20" si="3">((+O11*COS($N$3)-P11*SIN($N$3)+$N$7)*$R$3)</f>
         <v>127.712812921102</v>
       </c>
-      <c r="D11" s="24">
-        <f>((O11*SIN($N$3)+P11*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D11" s="23">
+        <f t="shared" ref="D11:D20" si="4">((O11*SIN($N$3)+P11*COS($N$3)+$N$9)*$R$4)</f>
         <v>-3.9999999999999858</v>
       </c>
-      <c r="E11" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M11/3.1416*180)+$N$5)</f>
+      <c r="E11" s="23">
+        <f t="shared" ref="E11:E20" si="5">IF(($R$3*$R$4)=1,1,-1)*(($M11/3.1416*180)+$N$5)</f>
         <v>-90</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
       </c>
-      <c r="G11" s="26">
-        <f t="shared" ref="G11:G20" si="3">IF($R$3*$R$4=-1,1,0)</f>
+      <c r="G11" s="25">
+        <f t="shared" ref="G11:G20" si="6">IF($R$3*$R$4=-1,1,0)</f>
         <v>1</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="42">
+      <c r="J11" s="41">
         <v>1</v>
       </c>
       <c r="K11" s="10">
@@ -4899,45 +4898,45 @@
       <c r="M11" s="6">
         <v>0</v>
       </c>
-      <c r="N11" s="57">
+      <c r="N11" s="56">
         <v>0</v>
       </c>
-      <c r="O11" s="43">
+      <c r="O11" s="42">
         <v>116</v>
       </c>
-      <c r="P11" s="44">
+      <c r="P11" s="43">
         <v>127.712812921102</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="C12" s="24">
-        <f>((+O12*COS($N$3)-P12*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C12" s="23">
+        <f t="shared" si="3"/>
         <v>136.95041722813599</v>
       </c>
-      <c r="D12" s="24">
-        <f>((O12*SIN($N$3)+P12*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D12" s="23">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="E12" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M12/3.1416*180)+$N$5)</f>
+      <c r="E12" s="23">
+        <f t="shared" si="5"/>
         <v>-30.000140305771573</v>
       </c>
       <c r="F12" s="11">
         <v>5</v>
       </c>
-      <c r="G12" s="26">
-        <f t="shared" si="3"/>
+      <c r="G12" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="42">
+      <c r="J12" s="41">
         <v>1</v>
       </c>
       <c r="K12" s="10">
@@ -4950,42 +4949,42 @@
         <v>-1.0471975511966001</v>
       </c>
       <c r="N12" s="4"/>
-      <c r="O12" s="43">
+      <c r="O12" s="42">
         <v>132</v>
       </c>
-      <c r="P12" s="44">
+      <c r="P12" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="C13" s="24">
-        <f>((+O13*COS($N$3)-P13*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C13" s="23">
+        <f t="shared" si="3"/>
         <v>155.425625842204</v>
       </c>
-      <c r="D13" s="24">
-        <f>((O13*SIN($N$3)+P13*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D13" s="23">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="E13" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M13/3.1416*180)+$N$5)</f>
+      <c r="E13" s="23">
+        <f t="shared" si="5"/>
         <v>-90</v>
       </c>
       <c r="F13" s="11">
         <v>5</v>
       </c>
-      <c r="G13" s="26">
-        <f t="shared" si="3"/>
+      <c r="G13" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="42">
+      <c r="J13" s="41">
         <v>1</v>
       </c>
       <c r="K13" s="10">
@@ -4998,42 +4997,42 @@
         <v>0</v>
       </c>
       <c r="N13" s="4"/>
-      <c r="O13" s="43">
+      <c r="O13" s="42">
         <v>132</v>
       </c>
-      <c r="P13" s="44">
+      <c r="P13" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C14" s="24">
-        <f>((+O14*COS($N$3)-P14*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C14" s="23">
+        <f t="shared" si="3"/>
         <v>164.66323014923799</v>
       </c>
-      <c r="D14" s="24">
-        <f>((O14*SIN($N$3)+P14*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D14" s="23">
+        <f t="shared" si="4"/>
         <v>-3.9999999999999858</v>
       </c>
-      <c r="E14" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M14/3.1416*180)+$N$5)</f>
+      <c r="E14" s="23">
+        <f t="shared" si="5"/>
         <v>-149.99985969422843</v>
       </c>
       <c r="F14" s="11">
         <v>5</v>
       </c>
-      <c r="G14" s="26">
-        <f t="shared" si="3"/>
+      <c r="G14" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="42">
+      <c r="J14" s="41">
         <v>1</v>
       </c>
       <c r="K14" s="10">
@@ -5046,42 +5045,42 @@
         <v>1.0471975511966001</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="43">
+      <c r="O14" s="42">
         <v>116</v>
       </c>
-      <c r="P14" s="44">
+      <c r="P14" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="C15" s="24">
-        <f>((+O15*COS($N$3)-P15*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C15" s="23">
+        <f t="shared" si="3"/>
         <v>183.138438763306</v>
       </c>
-      <c r="D15" s="24">
-        <f>((O15*SIN($N$3)+P15*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D15" s="23">
+        <f t="shared" si="4"/>
         <v>-3.9999999999999858</v>
       </c>
-      <c r="E15" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M15/3.1416*180)+$N$5)</f>
+      <c r="E15" s="23">
+        <f t="shared" si="5"/>
         <v>-90</v>
       </c>
       <c r="F15" s="11">
         <v>5</v>
       </c>
-      <c r="G15" s="26">
-        <f t="shared" si="3"/>
+      <c r="G15" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="42">
+      <c r="J15" s="41">
         <v>1</v>
       </c>
       <c r="K15" s="10">
@@ -5094,42 +5093,42 @@
         <v>0</v>
       </c>
       <c r="N15" s="4"/>
-      <c r="O15" s="43">
+      <c r="O15" s="42">
         <v>116</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="43">
         <v>183.138438763306</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="C16" s="24">
-        <f>((+O16*COS($N$3)-P16*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C16" s="23">
+        <f t="shared" si="3"/>
         <v>192.37604307033999</v>
       </c>
-      <c r="D16" s="24">
-        <f>((O16*SIN($N$3)+P16*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D16" s="23">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="E16" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M16/3.1416*180)+$N$5)</f>
+      <c r="E16" s="23">
+        <f t="shared" si="5"/>
         <v>-30.000140305771573</v>
       </c>
       <c r="F16" s="11">
         <v>5</v>
       </c>
-      <c r="G16" s="26">
-        <f t="shared" si="3"/>
+      <c r="G16" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="42">
+      <c r="J16" s="41">
         <v>1</v>
       </c>
       <c r="K16" s="10">
@@ -5142,42 +5141,42 @@
         <v>-1.0471975511966001</v>
       </c>
       <c r="N16" s="4"/>
-      <c r="O16" s="43">
+      <c r="O16" s="42">
         <v>132</v>
       </c>
-      <c r="P16" s="44">
+      <c r="P16" s="43">
         <v>192.37604307033999</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="C17" s="24">
-        <f>((+O17*COS($N$3)-P17*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C17" s="23">
+        <f t="shared" si="3"/>
         <v>192.37604307033999</v>
       </c>
-      <c r="D17" s="24">
-        <f>((O17*SIN($N$3)+P17*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D17" s="23">
+        <f t="shared" si="4"/>
         <v>-19.999999999999986</v>
       </c>
-      <c r="E17" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M17/3.1416*180)+$N$5)</f>
+      <c r="E17" s="23">
+        <f t="shared" si="5"/>
         <v>-149.99985969422843</v>
       </c>
       <c r="F17" s="11">
         <v>5</v>
       </c>
-      <c r="G17" s="26">
-        <f t="shared" si="3"/>
+      <c r="G17" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="42">
+      <c r="J17" s="41">
         <v>1</v>
       </c>
       <c r="K17" s="10">
@@ -5190,42 +5189,42 @@
         <v>1.0471975511966001</v>
       </c>
       <c r="N17" s="4"/>
-      <c r="O17" s="43">
+      <c r="O17" s="42">
         <v>100</v>
       </c>
-      <c r="P17" s="44">
+      <c r="P17" s="43">
         <v>192.37604307033999</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="C18" s="24">
-        <f>((+O18*COS($N$3)-P18*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C18" s="23">
+        <f t="shared" si="3"/>
         <v>183.138438763306</v>
       </c>
-      <c r="D18" s="24">
-        <f>((O18*SIN($N$3)+P18*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D18" s="23">
+        <f t="shared" si="4"/>
         <v>-35.999999999999986</v>
       </c>
-      <c r="E18" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M18/3.1416*180)+$N$5)</f>
-        <v>-90</v>
+      <c r="E18" s="23">
+        <f t="shared" si="5"/>
+        <v>-209.99971938845687</v>
       </c>
       <c r="F18" s="11">
         <v>5</v>
       </c>
-      <c r="G18" s="26">
-        <f t="shared" si="3"/>
+      <c r="G18" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="42">
+      <c r="J18" s="41">
         <v>1</v>
       </c>
       <c r="K18" s="10">
@@ -5235,45 +5234,45 @@
         <v>20</v>
       </c>
       <c r="M18" s="6">
-        <v>0</v>
+        <v>2.0943951023932001</v>
       </c>
       <c r="N18" s="4"/>
-      <c r="O18" s="43">
+      <c r="O18" s="42">
         <v>84</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="43">
         <v>183.138438763306</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="23">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="C19" s="24">
-        <f>((+O19*COS($N$3)-P19*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C19" s="23">
+        <f t="shared" si="3"/>
         <v>155.425625842204</v>
       </c>
-      <c r="D19" s="24">
-        <f>((O19*SIN($N$3)+P19*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D19" s="23">
+        <f t="shared" si="4"/>
         <v>-19.999999999999986</v>
       </c>
-      <c r="E19" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M19/3.1416*180)+$N$5)</f>
+      <c r="E19" s="23">
+        <f t="shared" si="5"/>
         <v>-209.99971938845687</v>
       </c>
       <c r="F19" s="11">
         <v>5</v>
       </c>
-      <c r="G19" s="26">
-        <f t="shared" si="3"/>
+      <c r="G19" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="42">
+      <c r="J19" s="41">
         <v>1</v>
       </c>
       <c r="K19" s="10">
@@ -5286,42 +5285,42 @@
         <v>2.0943951023932001</v>
       </c>
       <c r="N19" s="4"/>
-      <c r="O19" s="43">
+      <c r="O19" s="42">
         <v>100</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="23">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="C20" s="24">
-        <f>((+O20*COS($N$3)-P20*SIN($N$3)+$N$7)*$R$3)</f>
+      <c r="C20" s="23">
+        <f t="shared" si="3"/>
         <v>164.66323014923799</v>
       </c>
-      <c r="D20" s="24">
-        <f>((O20*SIN($N$3)+P20*COS($N$3)+$N$9)*$R$4)</f>
+      <c r="D20" s="23">
+        <f t="shared" si="4"/>
         <v>-35.999999999999986</v>
       </c>
-      <c r="E20" s="24">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M20/3.1416*180)+$N$5)</f>
+      <c r="E20" s="23">
+        <f t="shared" si="5"/>
         <v>-149.99985969422843</v>
       </c>
       <c r="F20" s="11">
         <v>5</v>
       </c>
-      <c r="G20" s="26">
-        <f t="shared" si="3"/>
+      <c r="G20" s="25">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="42">
+      <c r="J20" s="41">
         <v>1</v>
       </c>
       <c r="K20" s="10">
@@ -5334,23 +5333,23 @@
         <v>1.0471975511966001</v>
       </c>
       <c r="N20" s="4"/>
-      <c r="O20" s="43">
+      <c r="O20" s="42">
         <v>84</v>
       </c>
-      <c r="P20" s="44">
+      <c r="P20" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="26"/>
+      <c r="G21" s="25"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="42">
+      <c r="J21" s="41">
         <v>1</v>
       </c>
       <c r="K21" s="10">
@@ -5363,23 +5362,23 @@
         <v>2.0943951023932001</v>
       </c>
       <c r="N21" s="4"/>
-      <c r="O21" s="43">
+      <c r="O21" s="42">
         <v>68</v>
       </c>
-      <c r="P21" s="44">
+      <c r="P21" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="26"/>
+      <c r="G22" s="25"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="42">
+      <c r="J22" s="41">
         <v>1</v>
       </c>
       <c r="K22" s="10">
@@ -5392,42 +5391,42 @@
         <v>3.14159265358979</v>
       </c>
       <c r="N22" s="4"/>
-      <c r="O22" s="43">
+      <c r="O22" s="42">
         <v>68</v>
       </c>
-      <c r="P22" s="44">
+      <c r="P22" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="24">
-        <f t="shared" ref="B23:B25" si="4">((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
+      <c r="B23" s="23">
+        <f t="shared" ref="B23:B25" si="7">((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
         <v>11</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="23">
         <f>((+O23*COS($N$3)-P23*SIN($N$3)+$N$7)*$R$3)</f>
         <v>136.95041722813599</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="23">
         <f>((O23*SIN($N$3)+P23*COS($N$3)+$N$9)*$R$4)</f>
         <v>-19.999999999999986</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M23/3.1416*180)+$N$5)</f>
         <v>-269.9995790826847</v>
       </c>
       <c r="F23" s="11">
         <v>5</v>
       </c>
-      <c r="G23" s="26">
-        <f t="shared" ref="G23:G25" si="5">IF($R$3*$R$4=-1,1,0)</f>
+      <c r="G23" s="25">
+        <f t="shared" ref="G23:G25" si="8">IF($R$3*$R$4=-1,1,0)</f>
         <v>1</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="42">
+      <c r="J23" s="41">
         <v>1</v>
       </c>
       <c r="K23" s="10">
@@ -5440,42 +5439,42 @@
         <v>3.14159265358979</v>
       </c>
       <c r="N23" s="4"/>
-      <c r="O23" s="43">
+      <c r="O23" s="42">
         <v>100</v>
       </c>
-      <c r="P23" s="44">
+      <c r="P23" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="24">
-        <f t="shared" si="4"/>
+      <c r="B24" s="23">
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="23">
         <f>((+O24*COS($N$3)-P24*SIN($N$3)+$N$7)*$R$3)</f>
         <v>127.712812921102</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="23">
         <f>((O24*SIN($N$3)+P24*COS($N$3)+$N$9)*$R$4)</f>
         <v>-35.999999999999986</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M24/3.1416*180)+$N$5)</f>
         <v>-209.99971938845687</v>
       </c>
       <c r="F24" s="11">
         <v>5</v>
       </c>
-      <c r="G24" s="26">
-        <f t="shared" si="5"/>
+      <c r="G24" s="25">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="42">
+      <c r="J24" s="41">
         <v>1</v>
       </c>
       <c r="K24" s="10">
@@ -5488,58 +5487,58 @@
         <v>2.0943951023932001</v>
       </c>
       <c r="N24" s="4"/>
-      <c r="O24" s="43">
+      <c r="O24" s="42">
         <v>84</v>
       </c>
-      <c r="P24" s="44">
+      <c r="P24" s="43">
         <v>127.712812921102</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="24">
-        <f t="shared" si="4"/>
+      <c r="B25" s="23">
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="23">
         <f>((+O25*COS($N$3)-P25*SIN($N$3)+$N$7)*$R$3)</f>
         <v>109.237604307034</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="23">
         <f>((O25*SIN($N$3)+P25*COS($N$3)+$N$9)*$R$4)</f>
         <v>-36</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M25/3.1416*180)+$N$5)</f>
         <v>-269.9995790826847</v>
       </c>
       <c r="F25" s="11">
         <v>5</v>
       </c>
-      <c r="G25" s="26">
-        <f t="shared" si="5"/>
+      <c r="G25" s="25">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="42">
+      <c r="J25" s="41">
         <v>1</v>
       </c>
-      <c r="K25" s="46">
+      <c r="K25" s="45">
         <v>16</v>
       </c>
-      <c r="L25" s="47">
+      <c r="L25" s="46">
         <v>43</v>
       </c>
-      <c r="M25" s="48">
+      <c r="M25" s="47">
         <v>3.14159265358979</v>
       </c>
-      <c r="N25" s="49"/>
-      <c r="O25" s="50">
+      <c r="N25" s="48"/>
+      <c r="O25" s="49">
         <v>84</v>
       </c>
-      <c r="P25" s="51">
+      <c r="P25" s="50">
         <v>109.237604307034</v>
       </c>
     </row>
@@ -5807,7 +5806,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:G17"/>
+      <selection activeCell="M3" sqref="M3:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5833,81 +5832,81 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="56" t="s">
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="34" t="s">
+      <c r="P2" s="33" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="24">
-        <f t="shared" ref="B3:B4" si="0">((ROUND($L3/10,0))-1)*4+MOD($L3,10)+((J3-1)*16)</f>
+      <c r="B3" s="23">
+        <f t="shared" ref="B3" si="0">((ROUND($L3/10,0))-1)*4+MOD($L3,10)+((J3-1)*16)</f>
         <v>16</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <f>((+O3*COS($N$3)-P3*SIN($N$3)+$N$7)*$R$3)</f>
         <v>100</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <f>((O3*SIN($N$3)+P3*COS($N$3)+$N$9)*$R$4)</f>
         <v>-100</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)+$N$5)</f>
-        <v>-90</v>
+        <v>-209.99971938845687</v>
       </c>
       <c r="F3" s="11">
         <v>5</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <f t="shared" ref="G3:G4" si="1">IF($R$3*$R$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="40">
+      <c r="J3" s="39">
         <v>2</v>
       </c>
       <c r="K3" s="12">
@@ -5916,59 +5915,59 @@
       <c r="L3" s="13">
         <v>10</v>
       </c>
-      <c r="M3" s="14">
-        <v>0</v>
-      </c>
-      <c r="N3" s="15">
+      <c r="M3" s="6">
+        <v>-2.0943951023932001</v>
+      </c>
+      <c r="N3" s="14">
         <f>+RADIANS(N5)</f>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="15">
         <v>100</v>
       </c>
-      <c r="P3" s="41">
+      <c r="P3" s="40">
         <v>100</v>
       </c>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="53">
+      <c r="R3" s="52">
         <v>1</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <f t="shared" ref="B4" si="2">((ROUND($L4/10,0))-1)*4+MOD($L4,10)+((J4-1)*16)</f>
         <v>17</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <f>((+O4*COS($N$3)-P4*SIN($N$3)+$N$7)*$R$3)</f>
         <v>109.23760430703402</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <f>((O4*SIN($N$3)+P4*COS($N$3)+$N$9)*$R$4)</f>
         <v>-116</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M4/3.1416*180)+$N$5)</f>
         <v>-149.99985969422843</v>
       </c>
       <c r="F4" s="11">
         <v>5</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="40">
+      <c r="J4" s="39">
         <v>2</v>
       </c>
       <c r="K4" s="10">
@@ -5983,31 +5982,31 @@
       <c r="N4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="43">
+      <c r="O4" s="42">
         <v>116</v>
       </c>
-      <c r="P4" s="44">
+      <c r="P4" s="43">
         <v>109.237604307034</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="55">
+      <c r="R4" s="54">
         <v>1</v>
       </c>
       <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="26"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="40">
+      <c r="J5" s="39">
         <v>2</v>
       </c>
       <c r="K5" s="10">
@@ -6022,30 +6021,30 @@
       <c r="N5" s="3">
         <v>-90</v>
       </c>
-      <c r="O5" s="43">
+      <c r="O5" s="42">
         <v>132</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="43">
         <v>100</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="26"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="40">
+      <c r="J6" s="39">
         <v>2</v>
       </c>
       <c r="K6" s="10">
@@ -6057,31 +6056,31 @@
       <c r="M6" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N6" s="45" t="s">
+      <c r="N6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="43">
+      <c r="O6" s="42">
         <v>148</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="43">
         <v>109.237604307034</v>
       </c>
       <c r="S6" s="9"/>
-      <c r="T6" s="18" t="s">
+      <c r="T6" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="26"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="40">
+      <c r="J7" s="39">
         <v>2</v>
       </c>
       <c r="K7" s="10">
@@ -6096,27 +6095,27 @@
       <c r="N7" s="3">
         <v>0</v>
       </c>
-      <c r="O7" s="43">
+      <c r="O7" s="42">
         <v>148</v>
       </c>
-      <c r="P7" s="44">
+      <c r="P7" s="43">
         <v>127.712812921102</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="T7" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="26"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="40">
+      <c r="J8" s="39">
         <v>2</v>
       </c>
       <c r="K8" s="10">
@@ -6128,29 +6127,29 @@
       <c r="M8" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N8" s="45" t="s">
+      <c r="N8" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="43">
+      <c r="O8" s="42">
         <v>164</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="43">
         <v>136.95041722813599</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="26"/>
+      <c r="G9" s="25"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="40">
+      <c r="J9" s="39">
         <v>2</v>
       </c>
       <c r="K9" s="10">
@@ -6165,24 +6164,24 @@
       <c r="N9" s="3">
         <v>0</v>
       </c>
-      <c r="O9" s="43">
+      <c r="O9" s="42">
         <v>164</v>
       </c>
-      <c r="P9" s="44">
+      <c r="P9" s="43">
         <v>155.425625842204</v>
       </c>
       <c r="T9" s="7"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="26"/>
+      <c r="G10" s="25"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="40">
+      <c r="J10" s="39">
         <v>2</v>
       </c>
       <c r="K10" s="10">
@@ -6197,42 +6196,42 @@
       <c r="N10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="43">
+      <c r="O10" s="42">
         <v>148</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <f t="shared" ref="B11:B15" si="3">((ROUND($L11/10,0))-1)*4+MOD($L11,10)+((J11-1)*16)</f>
         <v>28</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="23">
         <f t="shared" ref="C11:C15" si="4">((+O11*COS($N$3)-P11*SIN($N$3)+$N$7)*$R$3)</f>
         <v>127.712812921102</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <f t="shared" ref="D11:D15" si="5">((O11*SIN($N$3)+P11*COS($N$3)+$N$9)*$R$4)</f>
         <v>-115.99999999999999</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="23">
         <f t="shared" ref="E11:E15" si="6">IF(($R$3*$R$4)=1,1,-1)*(($M11/3.1416*180)+$N$5)</f>
         <v>-90</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="25">
         <f t="shared" ref="G11:G15" si="7">IF($R$3*$R$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="40">
+      <c r="J11" s="39">
         <v>2</v>
       </c>
       <c r="K11" s="10">
@@ -6244,46 +6243,46 @@
       <c r="M11" s="6">
         <v>0</v>
       </c>
-      <c r="N11" s="57">
+      <c r="N11" s="56">
         <f>16*3</f>
         <v>48</v>
       </c>
-      <c r="O11" s="43">
+      <c r="O11" s="42">
         <v>116</v>
       </c>
-      <c r="P11" s="44">
+      <c r="P11" s="43">
         <v>127.712812921102</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="23">
         <f t="shared" si="4"/>
         <v>136.95041722813599</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="23">
         <f t="shared" si="5"/>
         <v>-132</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="23">
         <f t="shared" si="6"/>
         <v>-149.99985969422843</v>
       </c>
       <c r="F12" s="11">
         <v>5</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="25">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="40">
+      <c r="J12" s="39">
         <v>2</v>
       </c>
       <c r="K12" s="10">
@@ -6296,42 +6295,42 @@
         <v>-1.0471975511966001</v>
       </c>
       <c r="N12" s="4"/>
-      <c r="O12" s="43">
+      <c r="O12" s="42">
         <v>132</v>
       </c>
-      <c r="P12" s="44">
+      <c r="P12" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="23">
         <f t="shared" si="4"/>
         <v>155.425625842204</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="23">
         <f t="shared" si="5"/>
         <v>-132</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="23">
         <f t="shared" si="6"/>
         <v>-90</v>
       </c>
       <c r="F13" s="11">
         <v>5</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="25">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="40">
+      <c r="J13" s="39">
         <v>2</v>
       </c>
       <c r="K13" s="10">
@@ -6344,42 +6343,42 @@
         <v>0</v>
       </c>
       <c r="N13" s="4"/>
-      <c r="O13" s="43">
+      <c r="O13" s="42">
         <v>132</v>
       </c>
-      <c r="P13" s="44">
+      <c r="P13" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="23">
         <f t="shared" si="4"/>
         <v>164.66323014923799</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <f t="shared" si="5"/>
         <v>-115.99999999999999</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="23">
         <f t="shared" si="6"/>
         <v>-30.000140305771573</v>
       </c>
       <c r="F14" s="11">
         <v>5</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="25">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="40">
+      <c r="J14" s="39">
         <v>2</v>
       </c>
       <c r="K14" s="10">
@@ -6392,42 +6391,42 @@
         <v>1.0471975511966001</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="43">
+      <c r="O14" s="42">
         <v>116</v>
       </c>
-      <c r="P14" s="44">
+      <c r="P14" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="23">
         <f t="shared" si="4"/>
         <v>183.138438763306</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <f t="shared" si="5"/>
         <v>-115.99999999999999</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="23">
         <f t="shared" si="6"/>
         <v>-90</v>
       </c>
       <c r="F15" s="11">
         <v>5</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="25">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="40">
+      <c r="J15" s="39">
         <v>2</v>
       </c>
       <c r="K15" s="10">
@@ -6440,23 +6439,23 @@
         <v>0</v>
       </c>
       <c r="N15" s="4"/>
-      <c r="O15" s="43">
+      <c r="O15" s="42">
         <v>116</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="43">
         <v>183.138438763306</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="26"/>
+      <c r="G16" s="25"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="40">
+      <c r="J16" s="39">
         <v>2</v>
       </c>
       <c r="K16" s="10">
@@ -6469,42 +6468,42 @@
         <v>-1.0471975511966001</v>
       </c>
       <c r="N16" s="4"/>
-      <c r="O16" s="43">
+      <c r="O16" s="42">
         <v>132</v>
       </c>
-      <c r="P16" s="44">
+      <c r="P16" s="43">
         <v>192.37604307033999</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <f t="shared" ref="B17" si="8">((ROUND($L17/10,0))-1)*4+MOD($L17,10)+((J17-1)*16)</f>
         <v>19</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="23">
         <f>((+O17*COS($N$3)-P17*SIN($N$3)+$N$7)*$R$3)</f>
         <v>192.37604307033999</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <f>((O17*SIN($N$3)+P17*COS($N$3)+$N$9)*$R$4)</f>
         <v>-99.999999999999986</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="23">
         <f>IF(($R$3*$R$4)=1,1,-1)*(($M17/3.1416*180)+$N$5)</f>
         <v>-30.000140305771573</v>
       </c>
       <c r="F17" s="11">
         <v>5</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="25">
         <f t="shared" ref="G17" si="9">IF($R$3*$R$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="40">
+      <c r="J17" s="39">
         <v>2</v>
       </c>
       <c r="K17" s="10">
@@ -6517,23 +6516,23 @@
         <v>1.0471975511966001</v>
       </c>
       <c r="N17" s="4"/>
-      <c r="O17" s="43">
+      <c r="O17" s="42">
         <v>100</v>
       </c>
-      <c r="P17" s="44">
+      <c r="P17" s="43">
         <v>192.37604307033999</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="26"/>
+      <c r="G18" s="25"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="40">
+      <c r="J18" s="39">
         <v>2</v>
       </c>
       <c r="K18" s="10">
@@ -6543,26 +6542,26 @@
         <v>20</v>
       </c>
       <c r="M18" s="6">
-        <v>0</v>
+        <v>2.0943951023932001</v>
       </c>
       <c r="N18" s="4"/>
-      <c r="O18" s="43">
+      <c r="O18" s="42">
         <v>84</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="43">
         <v>183.138438763306</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="26"/>
+      <c r="G19" s="25"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="40">
+      <c r="J19" s="39">
         <v>2</v>
       </c>
       <c r="K19" s="10">
@@ -6575,23 +6574,23 @@
         <v>2.0943951023932001</v>
       </c>
       <c r="N19" s="4"/>
-      <c r="O19" s="43">
+      <c r="O19" s="42">
         <v>100</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="11"/>
-      <c r="G20" s="26"/>
+      <c r="G20" s="25"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="40">
+      <c r="J20" s="39">
         <v>2</v>
       </c>
       <c r="K20" s="10">
@@ -6604,23 +6603,23 @@
         <v>1.0471975511966001</v>
       </c>
       <c r="N20" s="4"/>
-      <c r="O20" s="43">
+      <c r="O20" s="42">
         <v>84</v>
       </c>
-      <c r="P20" s="44">
+      <c r="P20" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="26"/>
+      <c r="G21" s="25"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="40">
+      <c r="J21" s="39">
         <v>2</v>
       </c>
       <c r="K21" s="10">
@@ -6633,23 +6632,23 @@
         <v>2.0943951023932001</v>
       </c>
       <c r="N21" s="4"/>
-      <c r="O21" s="43">
+      <c r="O21" s="42">
         <v>68</v>
       </c>
-      <c r="P21" s="44">
+      <c r="P21" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="26"/>
+      <c r="G22" s="25"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="40">
+      <c r="J22" s="39">
         <v>2</v>
       </c>
       <c r="K22" s="10">
@@ -6662,23 +6661,23 @@
         <v>3.14159265358979</v>
       </c>
       <c r="N22" s="4"/>
-      <c r="O22" s="43">
+      <c r="O22" s="42">
         <v>68</v>
       </c>
-      <c r="P22" s="44">
+      <c r="P22" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="26"/>
+      <c r="G23" s="25"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="40">
+      <c r="J23" s="39">
         <v>2</v>
       </c>
       <c r="K23" s="10">
@@ -6691,23 +6690,23 @@
         <v>3.14159265358979</v>
       </c>
       <c r="N23" s="4"/>
-      <c r="O23" s="43">
+      <c r="O23" s="42">
         <v>100</v>
       </c>
-      <c r="P23" s="44">
+      <c r="P23" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="26"/>
+      <c r="G24" s="25"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="40">
+      <c r="J24" s="39">
         <v>2</v>
       </c>
       <c r="K24" s="10">
@@ -6720,39 +6719,39 @@
         <v>2.0943951023932001</v>
       </c>
       <c r="N24" s="4"/>
-      <c r="O24" s="43">
+      <c r="O24" s="42">
         <v>84</v>
       </c>
-      <c r="P24" s="44">
+      <c r="P24" s="43">
         <v>127.712812921102</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="30"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="40">
+      <c r="J25" s="39">
         <v>2</v>
       </c>
-      <c r="K25" s="46">
+      <c r="K25" s="45">
         <v>16</v>
       </c>
-      <c r="L25" s="47">
+      <c r="L25" s="46">
         <v>43</v>
       </c>
-      <c r="M25" s="48">
+      <c r="M25" s="47">
         <v>3.14159265358979</v>
       </c>
-      <c r="N25" s="49"/>
-      <c r="O25" s="50">
+      <c r="N25" s="48"/>
+      <c r="O25" s="49">
         <v>84</v>
       </c>
-      <c r="P25" s="51">
+      <c r="P25" s="50">
         <v>109.237604307034</v>
       </c>
     </row>
@@ -6771,1429 +6770,1429 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G48" sqref="A3:G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="62"/>
-    <col min="5" max="5" width="11.28515625" style="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="61"/>
+    <col min="5" max="5" width="11.28515625" style="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="38" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="str">
+      <c r="A3" s="57" t="str">
         <f>IF(lower!A3=0, "", lower!A3)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B3" s="61">
+      <c r="B3" s="60">
         <f>IF(lower!B3="", "", lower!B3)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="64">
+      <c r="C3" s="63">
         <f>IF(lower!C3="", "", lower!C3)</f>
         <v>100</v>
       </c>
-      <c r="D3" s="64">
+      <c r="D3" s="63">
         <f>IF(lower!D3="", "", lower!D3)</f>
         <v>-20</v>
       </c>
-      <c r="E3" s="64">
+      <c r="E3" s="63">
         <f>IF(lower!E3="", "", lower!E3)</f>
-        <v>-90</v>
-      </c>
-      <c r="F3" s="58">
+        <v>29.999719388456853</v>
+      </c>
+      <c r="F3" s="57">
         <f>IF(lower!F3=0, "", lower!F3)</f>
         <v>5</v>
       </c>
-      <c r="G3" s="58">
+      <c r="G3" s="57">
         <f>IF(lower!$A3=0, "", lower!G3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="str">
+      <c r="A4" s="57" t="str">
         <f>IF(lower!A4=0, "", lower!A4)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B4" s="61">
+      <c r="B4" s="60">
         <f>IF(lower!B4="", "", lower!B4)</f>
         <v>1</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="63">
         <f>IF(lower!C4="", "", lower!C4)</f>
         <v>109.23760430703399</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="63">
         <f>IF(lower!D4="", "", lower!D4)</f>
         <v>-4</v>
       </c>
-      <c r="E4" s="64">
+      <c r="E4" s="63">
         <f>IF(lower!E4="", "", lower!E4)</f>
         <v>-30.000140305771573</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="57">
         <f>IF(lower!F4=0, "", lower!F4)</f>
         <v>5</v>
       </c>
-      <c r="G4" s="58">
+      <c r="G4" s="57">
         <f>IF(lower!$A4=0, "", lower!G4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="str">
+      <c r="A5" s="57" t="str">
         <f>IF(lower!A5=0, "", lower!A5)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B5" s="61">
+      <c r="B5" s="60">
         <f>IF(lower!B5="", "", lower!B5)</f>
         <v>2</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="63">
         <f>IF(lower!C5="", "", lower!C5)</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="63">
         <f>IF(lower!D5="", "", lower!D5)</f>
         <v>12</v>
       </c>
-      <c r="E5" s="64">
+      <c r="E5" s="63">
         <f>IF(lower!E5="", "", lower!E5)</f>
         <v>29.999719388456853</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="57">
         <f>IF(lower!F5=0, "", lower!F5)</f>
         <v>5</v>
       </c>
-      <c r="G5" s="58">
+      <c r="G5" s="57">
         <f>IF(lower!$A5=0, "", lower!G5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="str">
+      <c r="A6" s="57" t="str">
         <f>IF(lower!A6=0, "", lower!A6)</f>
         <v/>
       </c>
-      <c r="B6" s="61" t="str">
+      <c r="B6" s="60" t="str">
         <f>IF(lower!B6="", "", lower!B6)</f>
         <v/>
       </c>
-      <c r="C6" s="64" t="str">
+      <c r="C6" s="63" t="str">
         <f>IF(lower!C6="", "", lower!C6)</f>
         <v/>
       </c>
-      <c r="D6" s="64" t="str">
+      <c r="D6" s="63" t="str">
         <f>IF(lower!D6="", "", lower!D6)</f>
         <v/>
       </c>
-      <c r="E6" s="64" t="str">
+      <c r="E6" s="63" t="str">
         <f>IF(lower!E6="", "", lower!E6)</f>
         <v/>
       </c>
-      <c r="F6" s="58" t="str">
+      <c r="F6" s="57" t="str">
         <f>IF(lower!F6=0, "", lower!F6)</f>
         <v/>
       </c>
-      <c r="G6" s="58" t="str">
+      <c r="G6" s="57" t="str">
         <f>IF(lower!$A6=0, "", lower!G6)</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="str">
+      <c r="A7" s="57" t="str">
         <f>IF(lower!A7=0, "", lower!A7)</f>
         <v/>
       </c>
-      <c r="B7" s="61" t="str">
+      <c r="B7" s="60" t="str">
         <f>IF(lower!B7="", "", lower!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="64" t="str">
+      <c r="C7" s="63" t="str">
         <f>IF(lower!C7="", "", lower!C7)</f>
         <v/>
       </c>
-      <c r="D7" s="64" t="str">
+      <c r="D7" s="63" t="str">
         <f>IF(lower!D7="", "", lower!D7)</f>
         <v/>
       </c>
-      <c r="E7" s="64" t="str">
+      <c r="E7" s="63" t="str">
         <f>IF(lower!E7="", "", lower!E7)</f>
         <v/>
       </c>
-      <c r="F7" s="58" t="str">
+      <c r="F7" s="57" t="str">
         <f>IF(lower!F7=0, "", lower!F7)</f>
         <v/>
       </c>
-      <c r="G7" s="58" t="str">
+      <c r="G7" s="57" t="str">
         <f>IF(lower!$A7=0, "", lower!G7)</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="str">
+      <c r="A8" s="57" t="str">
         <f>IF(lower!A8=0, "", lower!A8)</f>
         <v/>
       </c>
-      <c r="B8" s="61" t="str">
+      <c r="B8" s="60" t="str">
         <f>IF(lower!B8="", "", lower!B8)</f>
         <v/>
       </c>
-      <c r="C8" s="64" t="str">
+      <c r="C8" s="63" t="str">
         <f>IF(lower!C8="", "", lower!C8)</f>
         <v/>
       </c>
-      <c r="D8" s="64" t="str">
+      <c r="D8" s="63" t="str">
         <f>IF(lower!D8="", "", lower!D8)</f>
         <v/>
       </c>
-      <c r="E8" s="64" t="str">
+      <c r="E8" s="63" t="str">
         <f>IF(lower!E8="", "", lower!E8)</f>
         <v/>
       </c>
-      <c r="F8" s="58" t="str">
+      <c r="F8" s="57" t="str">
         <f>IF(lower!F8=0, "", lower!F8)</f>
         <v/>
       </c>
-      <c r="G8" s="58" t="str">
+      <c r="G8" s="57" t="str">
         <f>IF(lower!$A8=0, "", lower!G8)</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="str">
+      <c r="A9" s="57" t="str">
         <f>IF(lower!A9=0, "", lower!A9)</f>
         <v/>
       </c>
-      <c r="B9" s="61" t="str">
+      <c r="B9" s="60" t="str">
         <f>IF(lower!B9="", "", lower!B9)</f>
         <v/>
       </c>
-      <c r="C9" s="64" t="str">
+      <c r="C9" s="63" t="str">
         <f>IF(lower!C9="", "", lower!C9)</f>
         <v/>
       </c>
-      <c r="D9" s="64" t="str">
+      <c r="D9" s="63" t="str">
         <f>IF(lower!D9="", "", lower!D9)</f>
         <v/>
       </c>
-      <c r="E9" s="64" t="str">
+      <c r="E9" s="63" t="str">
         <f>IF(lower!E9="", "", lower!E9)</f>
         <v/>
       </c>
-      <c r="F9" s="58" t="str">
+      <c r="F9" s="57" t="str">
         <f>IF(lower!F9=0, "", lower!F9)</f>
         <v/>
       </c>
-      <c r="G9" s="58" t="str">
+      <c r="G9" s="57" t="str">
         <f>IF(lower!$A9=0, "", lower!G9)</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="str">
+      <c r="A10" s="57" t="str">
         <f>IF(lower!A10=0, "", lower!A10)</f>
         <v/>
       </c>
-      <c r="B10" s="61" t="str">
+      <c r="B10" s="60" t="str">
         <f>IF(lower!B10="", "", lower!B10)</f>
         <v/>
       </c>
-      <c r="C10" s="64" t="str">
+      <c r="C10" s="63" t="str">
         <f>IF(lower!C10="", "", lower!C10)</f>
         <v/>
       </c>
-      <c r="D10" s="64" t="str">
+      <c r="D10" s="63" t="str">
         <f>IF(lower!D10="", "", lower!D10)</f>
         <v/>
       </c>
-      <c r="E10" s="64" t="str">
+      <c r="E10" s="63" t="str">
         <f>IF(lower!E10="", "", lower!E10)</f>
         <v/>
       </c>
-      <c r="F10" s="58" t="str">
+      <c r="F10" s="57" t="str">
         <f>IF(lower!F10=0, "", lower!F10)</f>
         <v/>
       </c>
-      <c r="G10" s="58" t="str">
+      <c r="G10" s="57" t="str">
         <f>IF(lower!$A10=0, "", lower!G10)</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="str">
+      <c r="A11" s="57" t="str">
         <f>IF(lower!A11=0, "", lower!A11)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B11" s="61">
+      <c r="B11" s="60">
         <f>IF(lower!B11="", "", lower!B11)</f>
         <v>12</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="63">
         <f>IF(lower!C11="", "", lower!C11)</f>
         <v>127.712812921102</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="63">
         <f>IF(lower!D11="", "", lower!D11)</f>
         <v>-3.9999999999999858</v>
       </c>
-      <c r="E11" s="64">
+      <c r="E11" s="63">
         <f>IF(lower!E11="", "", lower!E11)</f>
         <v>-90</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="57">
         <f>IF(lower!F11=0, "", lower!F11)</f>
         <v>5</v>
       </c>
-      <c r="G11" s="58">
+      <c r="G11" s="57">
         <f>IF(lower!$A11=0, "", lower!G11)</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="str">
+      <c r="A12" s="57" t="str">
         <f>IF(lower!A12=0, "", lower!A12)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B12" s="61">
+      <c r="B12" s="60">
         <f>IF(lower!B12="", "", lower!B12)</f>
         <v>13</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="63">
         <f>IF(lower!C12="", "", lower!C12)</f>
         <v>136.95041722813599</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="63">
         <f>IF(lower!D12="", "", lower!D12)</f>
         <v>12</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="63">
         <f>IF(lower!E12="", "", lower!E12)</f>
         <v>-30.000140305771573</v>
       </c>
-      <c r="F12" s="58">
+      <c r="F12" s="57">
         <f>IF(lower!F12=0, "", lower!F12)</f>
         <v>5</v>
       </c>
-      <c r="G12" s="58">
+      <c r="G12" s="57">
         <f>IF(lower!$A12=0, "", lower!G12)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="str">
+      <c r="A13" s="57" t="str">
         <f>IF(lower!A13=0, "", lower!A13)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B13" s="61">
+      <c r="B13" s="60">
         <f>IF(lower!B13="", "", lower!B13)</f>
         <v>8</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="63">
         <f>IF(lower!C13="", "", lower!C13)</f>
         <v>155.425625842204</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="63">
         <f>IF(lower!D13="", "", lower!D13)</f>
         <v>12</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="63">
         <f>IF(lower!E13="", "", lower!E13)</f>
         <v>-90</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="57">
         <f>IF(lower!F13=0, "", lower!F13)</f>
         <v>5</v>
       </c>
-      <c r="G13" s="58">
+      <c r="G13" s="57">
         <f>IF(lower!$A13=0, "", lower!G13)</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="str">
+      <c r="A14" s="57" t="str">
         <f>IF(lower!A14=0, "", lower!A14)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B14" s="61">
+      <c r="B14" s="60">
         <f>IF(lower!B14="", "", lower!B14)</f>
         <v>9</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="63">
         <f>IF(lower!C14="", "", lower!C14)</f>
         <v>164.66323014923799</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="63">
         <f>IF(lower!D14="", "", lower!D14)</f>
         <v>-3.9999999999999858</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="63">
         <f>IF(lower!E14="", "", lower!E14)</f>
         <v>-149.99985969422843</v>
       </c>
-      <c r="F14" s="58">
+      <c r="F14" s="57">
         <f>IF(lower!F14=0, "", lower!F14)</f>
         <v>5</v>
       </c>
-      <c r="G14" s="58">
+      <c r="G14" s="57">
         <f>IF(lower!$A14=0, "", lower!G14)</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="str">
+      <c r="A15" s="57" t="str">
         <f>IF(lower!A15=0, "", lower!A15)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B15" s="61">
+      <c r="B15" s="60">
         <f>IF(lower!B15="", "", lower!B15)</f>
         <v>6</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="63">
         <f>IF(lower!C15="", "", lower!C15)</f>
         <v>183.138438763306</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="63">
         <f>IF(lower!D15="", "", lower!D15)</f>
         <v>-3.9999999999999858</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="63">
         <f>IF(lower!E15="", "", lower!E15)</f>
         <v>-90</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="57">
         <f>IF(lower!F15=0, "", lower!F15)</f>
         <v>5</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="57">
         <f>IF(lower!$A15=0, "", lower!G15)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="str">
+      <c r="A16" s="57" t="str">
         <f>IF(lower!A16=0, "", lower!A16)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B16" s="61">
+      <c r="B16" s="60">
         <f>IF(lower!B16="", "", lower!B16)</f>
         <v>7</v>
       </c>
-      <c r="C16" s="64">
+      <c r="C16" s="63">
         <f>IF(lower!C16="", "", lower!C16)</f>
         <v>192.37604307033999</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="63">
         <f>IF(lower!D16="", "", lower!D16)</f>
         <v>12</v>
       </c>
-      <c r="E16" s="64">
+      <c r="E16" s="63">
         <f>IF(lower!E16="", "", lower!E16)</f>
         <v>-30.000140305771573</v>
       </c>
-      <c r="F16" s="58">
+      <c r="F16" s="57">
         <f>IF(lower!F16=0, "", lower!F16)</f>
         <v>5</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="57">
         <f>IF(lower!$A16=0, "", lower!G16)</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="58" t="str">
+      <c r="A17" s="57" t="str">
         <f>IF(lower!A17=0, "", lower!A17)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B17" s="61">
+      <c r="B17" s="60">
         <f>IF(lower!B17="", "", lower!B17)</f>
         <v>3</v>
       </c>
-      <c r="C17" s="64">
+      <c r="C17" s="63">
         <f>IF(lower!C17="", "", lower!C17)</f>
         <v>192.37604307033999</v>
       </c>
-      <c r="D17" s="64">
+      <c r="D17" s="63">
         <f>IF(lower!D17="", "", lower!D17)</f>
         <v>-19.999999999999986</v>
       </c>
-      <c r="E17" s="64">
+      <c r="E17" s="63">
         <f>IF(lower!E17="", "", lower!E17)</f>
         <v>-149.99985969422843</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="57">
         <f>IF(lower!F17=0, "", lower!F17)</f>
         <v>5</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="57">
         <f>IF(lower!$A17=0, "", lower!G17)</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="str">
+      <c r="A18" s="57" t="str">
         <f>IF(lower!A18=0, "", lower!A18)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B18" s="61">
+      <c r="B18" s="60">
         <f>IF(lower!B18="", "", lower!B18)</f>
         <v>4</v>
       </c>
-      <c r="C18" s="64">
+      <c r="C18" s="63">
         <f>IF(lower!C18="", "", lower!C18)</f>
         <v>183.138438763306</v>
       </c>
-      <c r="D18" s="64">
+      <c r="D18" s="63">
         <f>IF(lower!D18="", "", lower!D18)</f>
         <v>-35.999999999999986</v>
       </c>
-      <c r="E18" s="64">
+      <c r="E18" s="63">
         <f>IF(lower!E18="", "", lower!E18)</f>
-        <v>-90</v>
-      </c>
-      <c r="F18" s="58">
+        <v>-209.99971938845687</v>
+      </c>
+      <c r="F18" s="57">
         <f>IF(lower!F18=0, "", lower!F18)</f>
         <v>5</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="57">
         <f>IF(lower!$A18=0, "", lower!G18)</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="str">
+      <c r="A19" s="57" t="str">
         <f>IF(lower!A19=0, "", lower!A19)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B19" s="61">
+      <c r="B19" s="60">
         <f>IF(lower!B19="", "", lower!B19)</f>
         <v>10</v>
       </c>
-      <c r="C19" s="64">
+      <c r="C19" s="63">
         <f>IF(lower!C19="", "", lower!C19)</f>
         <v>155.425625842204</v>
       </c>
-      <c r="D19" s="64">
+      <c r="D19" s="63">
         <f>IF(lower!D19="", "", lower!D19)</f>
         <v>-19.999999999999986</v>
       </c>
-      <c r="E19" s="64">
+      <c r="E19" s="63">
         <f>IF(lower!E19="", "", lower!E19)</f>
         <v>-209.99971938845687</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="57">
         <f>IF(lower!F19=0, "", lower!F19)</f>
         <v>5</v>
       </c>
-      <c r="G19" s="58">
+      <c r="G19" s="57">
         <f>IF(lower!$A19=0, "", lower!G19)</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="58" t="str">
+      <c r="A20" s="57" t="str">
         <f>IF(lower!A20=0, "", lower!A20)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B20" s="61">
+      <c r="B20" s="60">
         <f>IF(lower!B20="", "", lower!B20)</f>
         <v>5</v>
       </c>
-      <c r="C20" s="64">
+      <c r="C20" s="63">
         <f>IF(lower!C20="", "", lower!C20)</f>
         <v>164.66323014923799</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="63">
         <f>IF(lower!D20="", "", lower!D20)</f>
         <v>-35.999999999999986</v>
       </c>
-      <c r="E20" s="64">
+      <c r="E20" s="63">
         <f>IF(lower!E20="", "", lower!E20)</f>
         <v>-149.99985969422843</v>
       </c>
-      <c r="F20" s="58">
+      <c r="F20" s="57">
         <f>IF(lower!F20=0, "", lower!F20)</f>
         <v>5</v>
       </c>
-      <c r="G20" s="58">
+      <c r="G20" s="57">
         <f>IF(lower!$A20=0, "", lower!G20)</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="str">
+      <c r="A21" s="57" t="str">
         <f>IF(lower!A21=0, "", lower!A21)</f>
         <v/>
       </c>
-      <c r="B21" s="61" t="str">
+      <c r="B21" s="60" t="str">
         <f>IF(lower!B21="", "", lower!B21)</f>
         <v/>
       </c>
-      <c r="C21" s="64" t="str">
+      <c r="C21" s="63" t="str">
         <f>IF(lower!C21="", "", lower!C21)</f>
         <v/>
       </c>
-      <c r="D21" s="64" t="str">
+      <c r="D21" s="63" t="str">
         <f>IF(lower!D21="", "", lower!D21)</f>
         <v/>
       </c>
-      <c r="E21" s="64" t="str">
+      <c r="E21" s="63" t="str">
         <f>IF(lower!E21="", "", lower!E21)</f>
         <v/>
       </c>
-      <c r="F21" s="58" t="str">
+      <c r="F21" s="57" t="str">
         <f>IF(lower!F21=0, "", lower!F21)</f>
         <v/>
       </c>
-      <c r="G21" s="58" t="str">
+      <c r="G21" s="57" t="str">
         <f>IF(lower!$A21=0, "", lower!G21)</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="str">
+      <c r="A22" s="57" t="str">
         <f>IF(lower!A22=0, "", lower!A22)</f>
         <v/>
       </c>
-      <c r="B22" s="61" t="str">
+      <c r="B22" s="60" t="str">
         <f>IF(lower!B22="", "", lower!B22)</f>
         <v/>
       </c>
-      <c r="C22" s="64" t="str">
+      <c r="C22" s="63" t="str">
         <f>IF(lower!C22="", "", lower!C22)</f>
         <v/>
       </c>
-      <c r="D22" s="64" t="str">
+      <c r="D22" s="63" t="str">
         <f>IF(lower!D22="", "", lower!D22)</f>
         <v/>
       </c>
-      <c r="E22" s="64" t="str">
+      <c r="E22" s="63" t="str">
         <f>IF(lower!E22="", "", lower!E22)</f>
         <v/>
       </c>
-      <c r="F22" s="58" t="str">
+      <c r="F22" s="57" t="str">
         <f>IF(lower!F22=0, "", lower!F22)</f>
         <v/>
       </c>
-      <c r="G22" s="58" t="str">
+      <c r="G22" s="57" t="str">
         <f>IF(lower!$A22=0, "", lower!G22)</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="str">
+      <c r="A23" s="57" t="str">
         <f>IF(lower!A23=0, "", lower!A23)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B23" s="61">
+      <c r="B23" s="60">
         <f>IF(lower!B23="", "", lower!B23)</f>
         <v>11</v>
       </c>
-      <c r="C23" s="64">
+      <c r="C23" s="63">
         <f>IF(lower!C23="", "", lower!C23)</f>
         <v>136.95041722813599</v>
       </c>
-      <c r="D23" s="64">
+      <c r="D23" s="63">
         <f>IF(lower!D23="", "", lower!D23)</f>
         <v>-19.999999999999986</v>
       </c>
-      <c r="E23" s="64">
+      <c r="E23" s="63">
         <f>IF(lower!E23="", "", lower!E23)</f>
         <v>-269.9995790826847</v>
       </c>
-      <c r="F23" s="58">
+      <c r="F23" s="57">
         <f>IF(lower!F23=0, "", lower!F23)</f>
         <v>5</v>
       </c>
-      <c r="G23" s="58">
+      <c r="G23" s="57">
         <f>IF(lower!$A23=0, "", lower!G23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="str">
+      <c r="A24" s="57" t="str">
         <f>IF(lower!A24=0, "", lower!A24)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B24" s="61">
+      <c r="B24" s="60">
         <f>IF(lower!B24="", "", lower!B24)</f>
         <v>14</v>
       </c>
-      <c r="C24" s="64">
+      <c r="C24" s="63">
         <f>IF(lower!C24="", "", lower!C24)</f>
         <v>127.712812921102</v>
       </c>
-      <c r="D24" s="64">
+      <c r="D24" s="63">
         <f>IF(lower!D24="", "", lower!D24)</f>
         <v>-35.999999999999986</v>
       </c>
-      <c r="E24" s="64">
+      <c r="E24" s="63">
         <f>IF(lower!E24="", "", lower!E24)</f>
         <v>-209.99971938845687</v>
       </c>
-      <c r="F24" s="58">
+      <c r="F24" s="57">
         <f>IF(lower!F24=0, "", lower!F24)</f>
         <v>5</v>
       </c>
-      <c r="G24" s="58">
+      <c r="G24" s="57">
         <f>IF(lower!$A24=0, "", lower!G24)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="str">
+      <c r="A25" s="57" t="str">
         <f>IF(lower!A25=0, "", lower!A25)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B25" s="61">
+      <c r="B25" s="60">
         <f>IF(lower!B25="", "", lower!B25)</f>
         <v>15</v>
       </c>
-      <c r="C25" s="64">
+      <c r="C25" s="63">
         <f>IF(lower!C25="", "", lower!C25)</f>
         <v>109.237604307034</v>
       </c>
-      <c r="D25" s="64">
+      <c r="D25" s="63">
         <f>IF(lower!D25="", "", lower!D25)</f>
         <v>-36</v>
       </c>
-      <c r="E25" s="64">
+      <c r="E25" s="63">
         <f>IF(lower!E25="", "", lower!E25)</f>
         <v>-269.9995790826847</v>
       </c>
-      <c r="F25" s="58">
+      <c r="F25" s="57">
         <f>IF(lower!F25=0, "", lower!F25)</f>
         <v>5</v>
       </c>
-      <c r="G25" s="58">
+      <c r="G25" s="57">
         <f>IF(lower!$A25=0, "", lower!G25)</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="59" t="str">
+      <c r="A26" s="58" t="str">
         <f>IF(upper!A3=0, "", upper!A3)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B26" s="59">
+      <c r="B26" s="58">
         <f>IF(upper!B3="", "", upper!B3)</f>
         <v>16</v>
       </c>
-      <c r="C26" s="65">
+      <c r="C26" s="64">
         <f>IF(upper!C3="", "", upper!C3)</f>
         <v>100</v>
       </c>
-      <c r="D26" s="65">
+      <c r="D26" s="64">
         <f>IF(upper!D3="", "", upper!D3)</f>
         <v>-100</v>
       </c>
-      <c r="E26" s="65">
+      <c r="E26" s="64">
         <f>IF(upper!E3="", "", upper!E3)</f>
-        <v>-90</v>
-      </c>
-      <c r="F26" s="59">
+        <v>-209.99971938845687</v>
+      </c>
+      <c r="F26" s="58">
         <f>IF(upper!F3=0, "", upper!F3)</f>
         <v>5</v>
       </c>
-      <c r="G26" s="59">
+      <c r="G26" s="58">
         <f>IF(upper!A3=0, "", upper!G3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="59" t="str">
+      <c r="A27" s="58" t="str">
         <f>IF(upper!A4=0, "", upper!A4)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B27" s="59">
+      <c r="B27" s="58">
         <f>IF(upper!B4="", "", upper!B4)</f>
         <v>17</v>
       </c>
-      <c r="C27" s="65">
+      <c r="C27" s="64">
         <f>IF(upper!C4="", "", upper!C4)</f>
         <v>109.23760430703402</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D27" s="64">
         <f>IF(upper!D4="", "", upper!D4)</f>
         <v>-116</v>
       </c>
-      <c r="E27" s="65">
+      <c r="E27" s="64">
         <f>IF(upper!E4="", "", upper!E4)</f>
         <v>-149.99985969422843</v>
       </c>
-      <c r="F27" s="59">
+      <c r="F27" s="58">
         <f>IF(upper!F4=0, "", upper!F4)</f>
         <v>5</v>
       </c>
-      <c r="G27" s="59">
+      <c r="G27" s="58">
         <f>IF(upper!A4=0, "", upper!G4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="str">
+      <c r="A28" s="58" t="str">
         <f>IF(upper!A5=0, "", upper!A5)</f>
         <v/>
       </c>
-      <c r="B28" s="59" t="str">
+      <c r="B28" s="58" t="str">
         <f>IF(upper!B5="", "", upper!B5)</f>
         <v/>
       </c>
-      <c r="C28" s="65" t="str">
+      <c r="C28" s="64" t="str">
         <f>IF(upper!C5="", "", upper!C5)</f>
         <v/>
       </c>
-      <c r="D28" s="65" t="str">
+      <c r="D28" s="64" t="str">
         <f>IF(upper!D5="", "", upper!D5)</f>
         <v/>
       </c>
-      <c r="E28" s="65" t="str">
+      <c r="E28" s="64" t="str">
         <f>IF(upper!E5="", "", upper!E5)</f>
         <v/>
       </c>
-      <c r="F28" s="59" t="str">
+      <c r="F28" s="58" t="str">
         <f>IF(upper!F5=0, "", upper!F5)</f>
         <v/>
       </c>
-      <c r="G28" s="59" t="str">
+      <c r="G28" s="58" t="str">
         <f>IF(upper!A5=0, "", upper!G5)</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="59" t="str">
+      <c r="A29" s="58" t="str">
         <f>IF(upper!A6=0, "", upper!A6)</f>
         <v/>
       </c>
-      <c r="B29" s="59" t="str">
+      <c r="B29" s="58" t="str">
         <f>IF(upper!B6="", "", upper!B6)</f>
         <v/>
       </c>
-      <c r="C29" s="65" t="str">
+      <c r="C29" s="64" t="str">
         <f>IF(upper!C6="", "", upper!C6)</f>
         <v/>
       </c>
-      <c r="D29" s="65" t="str">
+      <c r="D29" s="64" t="str">
         <f>IF(upper!D6="", "", upper!D6)</f>
         <v/>
       </c>
-      <c r="E29" s="65" t="str">
+      <c r="E29" s="64" t="str">
         <f>IF(upper!E6="", "", upper!E6)</f>
         <v/>
       </c>
-      <c r="F29" s="59" t="str">
+      <c r="F29" s="58" t="str">
         <f>IF(upper!F6=0, "", upper!F6)</f>
         <v/>
       </c>
-      <c r="G29" s="59" t="str">
+      <c r="G29" s="58" t="str">
         <f>IF(upper!A6=0, "", upper!G6)</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="59" t="str">
+      <c r="A30" s="58" t="str">
         <f>IF(upper!A7=0, "", upper!A7)</f>
         <v/>
       </c>
-      <c r="B30" s="59" t="str">
+      <c r="B30" s="58" t="str">
         <f>IF(upper!B7="", "", upper!B7)</f>
         <v/>
       </c>
-      <c r="C30" s="65" t="str">
+      <c r="C30" s="64" t="str">
         <f>IF(upper!C7="", "", upper!C7)</f>
         <v/>
       </c>
-      <c r="D30" s="65" t="str">
+      <c r="D30" s="64" t="str">
         <f>IF(upper!D7="", "", upper!D7)</f>
         <v/>
       </c>
-      <c r="E30" s="65" t="str">
+      <c r="E30" s="64" t="str">
         <f>IF(upper!E7="", "", upper!E7)</f>
         <v/>
       </c>
-      <c r="F30" s="59" t="str">
+      <c r="F30" s="58" t="str">
         <f>IF(upper!F7=0, "", upper!F7)</f>
         <v/>
       </c>
-      <c r="G30" s="59" t="str">
+      <c r="G30" s="58" t="str">
         <f>IF(upper!A7=0, "", upper!G7)</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="59" t="str">
+      <c r="A31" s="58" t="str">
         <f>IF(upper!A8=0, "", upper!A8)</f>
         <v/>
       </c>
-      <c r="B31" s="59" t="str">
+      <c r="B31" s="58" t="str">
         <f>IF(upper!B8="", "", upper!B8)</f>
         <v/>
       </c>
-      <c r="C31" s="65" t="str">
+      <c r="C31" s="64" t="str">
         <f>IF(upper!C8="", "", upper!C8)</f>
         <v/>
       </c>
-      <c r="D31" s="65" t="str">
+      <c r="D31" s="64" t="str">
         <f>IF(upper!D8="", "", upper!D8)</f>
         <v/>
       </c>
-      <c r="E31" s="65" t="str">
+      <c r="E31" s="64" t="str">
         <f>IF(upper!E8="", "", upper!E8)</f>
         <v/>
       </c>
-      <c r="F31" s="59" t="str">
+      <c r="F31" s="58" t="str">
         <f>IF(upper!F8=0, "", upper!F8)</f>
         <v/>
       </c>
-      <c r="G31" s="59" t="str">
+      <c r="G31" s="58" t="str">
         <f>IF(upper!A8=0, "", upper!G8)</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="59" t="str">
+      <c r="A32" s="58" t="str">
         <f>IF(upper!A9=0, "", upper!A9)</f>
         <v/>
       </c>
-      <c r="B32" s="59" t="str">
+      <c r="B32" s="58" t="str">
         <f>IF(upper!B9="", "", upper!B9)</f>
         <v/>
       </c>
-      <c r="C32" s="65" t="str">
+      <c r="C32" s="64" t="str">
         <f>IF(upper!C9="", "", upper!C9)</f>
         <v/>
       </c>
-      <c r="D32" s="65" t="str">
+      <c r="D32" s="64" t="str">
         <f>IF(upper!D9="", "", upper!D9)</f>
         <v/>
       </c>
-      <c r="E32" s="65" t="str">
+      <c r="E32" s="64" t="str">
         <f>IF(upper!E9="", "", upper!E9)</f>
         <v/>
       </c>
-      <c r="F32" s="59" t="str">
+      <c r="F32" s="58" t="str">
         <f>IF(upper!F9=0, "", upper!F9)</f>
         <v/>
       </c>
-      <c r="G32" s="59" t="str">
+      <c r="G32" s="58" t="str">
         <f>IF(upper!A9=0, "", upper!G9)</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="59" t="str">
+      <c r="A33" s="58" t="str">
         <f>IF(upper!A10=0, "", upper!A10)</f>
         <v/>
       </c>
-      <c r="B33" s="59" t="str">
+      <c r="B33" s="58" t="str">
         <f>IF(upper!B10="", "", upper!B10)</f>
         <v/>
       </c>
-      <c r="C33" s="65" t="str">
+      <c r="C33" s="64" t="str">
         <f>IF(upper!C10="", "", upper!C10)</f>
         <v/>
       </c>
-      <c r="D33" s="65" t="str">
+      <c r="D33" s="64" t="str">
         <f>IF(upper!D10="", "", upper!D10)</f>
         <v/>
       </c>
-      <c r="E33" s="65" t="str">
+      <c r="E33" s="64" t="str">
         <f>IF(upper!E10="", "", upper!E10)</f>
         <v/>
       </c>
-      <c r="F33" s="59" t="str">
+      <c r="F33" s="58" t="str">
         <f>IF(upper!F10=0, "", upper!F10)</f>
         <v/>
       </c>
-      <c r="G33" s="59" t="str">
+      <c r="G33" s="58" t="str">
         <f>IF(upper!A10=0, "", upper!G10)</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="59" t="str">
+      <c r="A34" s="58" t="str">
         <f>IF(upper!A11=0, "", upper!A11)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B34" s="59">
+      <c r="B34" s="58">
         <f>IF(upper!B11="", "", upper!B11)</f>
         <v>28</v>
       </c>
-      <c r="C34" s="65">
+      <c r="C34" s="64">
         <f>IF(upper!C11="", "", upper!C11)</f>
         <v>127.712812921102</v>
       </c>
-      <c r="D34" s="65">
+      <c r="D34" s="64">
         <f>IF(upper!D11="", "", upper!D11)</f>
         <v>-115.99999999999999</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="64">
         <f>IF(upper!E11="", "", upper!E11)</f>
         <v>-90</v>
       </c>
-      <c r="F34" s="59">
+      <c r="F34" s="58">
         <f>IF(upper!F11=0, "", upper!F11)</f>
         <v>5</v>
       </c>
-      <c r="G34" s="59">
+      <c r="G34" s="58">
         <f>IF(upper!A11=0, "", upper!G11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="59" t="str">
+      <c r="A35" s="58" t="str">
         <f>IF(upper!A12=0, "", upper!A12)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B35" s="59">
+      <c r="B35" s="58">
         <f>IF(upper!B12="", "", upper!B12)</f>
         <v>29</v>
       </c>
-      <c r="C35" s="65">
+      <c r="C35" s="64">
         <f>IF(upper!C12="", "", upper!C12)</f>
         <v>136.95041722813599</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="64">
         <f>IF(upper!D12="", "", upper!D12)</f>
         <v>-132</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="64">
         <f>IF(upper!E12="", "", upper!E12)</f>
         <v>-149.99985969422843</v>
       </c>
-      <c r="F35" s="59">
+      <c r="F35" s="58">
         <f>IF(upper!F12=0, "", upper!F12)</f>
         <v>5</v>
       </c>
-      <c r="G35" s="59">
+      <c r="G35" s="58">
         <f>IF(upper!A12=0, "", upper!G12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="59" t="str">
+      <c r="A36" s="58" t="str">
         <f>IF(upper!A13=0, "", upper!A13)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B36" s="59">
+      <c r="B36" s="58">
         <f>IF(upper!B13="", "", upper!B13)</f>
         <v>24</v>
       </c>
-      <c r="C36" s="65">
+      <c r="C36" s="64">
         <f>IF(upper!C13="", "", upper!C13)</f>
         <v>155.425625842204</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="64">
         <f>IF(upper!D13="", "", upper!D13)</f>
         <v>-132</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="64">
         <f>IF(upper!E13="", "", upper!E13)</f>
         <v>-90</v>
       </c>
-      <c r="F36" s="59">
+      <c r="F36" s="58">
         <f>IF(upper!F13=0, "", upper!F13)</f>
         <v>5</v>
       </c>
-      <c r="G36" s="59">
+      <c r="G36" s="58">
         <f>IF(upper!A13=0, "", upper!G13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="59" t="str">
+      <c r="A37" s="58" t="str">
         <f>IF(upper!A14=0, "", upper!A14)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B37" s="59">
+      <c r="B37" s="58">
         <f>IF(upper!B14="", "", upper!B14)</f>
         <v>25</v>
       </c>
-      <c r="C37" s="65">
+      <c r="C37" s="64">
         <f>IF(upper!C14="", "", upper!C14)</f>
         <v>164.66323014923799</v>
       </c>
-      <c r="D37" s="65">
+      <c r="D37" s="64">
         <f>IF(upper!D14="", "", upper!D14)</f>
         <v>-115.99999999999999</v>
       </c>
-      <c r="E37" s="65">
+      <c r="E37" s="64">
         <f>IF(upper!E14="", "", upper!E14)</f>
         <v>-30.000140305771573</v>
       </c>
-      <c r="F37" s="59">
+      <c r="F37" s="58">
         <f>IF(upper!F14=0, "", upper!F14)</f>
         <v>5</v>
       </c>
-      <c r="G37" s="59">
+      <c r="G37" s="58">
         <f>IF(upper!A14=0, "", upper!G14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="59" t="str">
+      <c r="A38" s="58" t="str">
         <f>IF(upper!A15=0, "", upper!A15)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B38" s="59">
+      <c r="B38" s="58">
         <f>IF(upper!B15="", "", upper!B15)</f>
         <v>22</v>
       </c>
-      <c r="C38" s="65">
+      <c r="C38" s="64">
         <f>IF(upper!C15="", "", upper!C15)</f>
         <v>183.138438763306</v>
       </c>
-      <c r="D38" s="65">
+      <c r="D38" s="64">
         <f>IF(upper!D15="", "", upper!D15)</f>
         <v>-115.99999999999999</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="64">
         <f>IF(upper!E15="", "", upper!E15)</f>
         <v>-90</v>
       </c>
-      <c r="F38" s="59">
+      <c r="F38" s="58">
         <f>IF(upper!F15=0, "", upper!F15)</f>
         <v>5</v>
       </c>
-      <c r="G38" s="59">
+      <c r="G38" s="58">
         <f>IF(upper!A15=0, "", upper!G15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="59" t="str">
+      <c r="A39" s="58" t="str">
         <f>IF(upper!A16=0, "", upper!A16)</f>
         <v/>
       </c>
-      <c r="B39" s="59" t="str">
+      <c r="B39" s="58" t="str">
         <f>IF(upper!B16="", "", upper!B16)</f>
         <v/>
       </c>
-      <c r="C39" s="65" t="str">
+      <c r="C39" s="64" t="str">
         <f>IF(upper!C16="", "", upper!C16)</f>
         <v/>
       </c>
-      <c r="D39" s="65" t="str">
+      <c r="D39" s="64" t="str">
         <f>IF(upper!D16="", "", upper!D16)</f>
         <v/>
       </c>
-      <c r="E39" s="65" t="str">
+      <c r="E39" s="64" t="str">
         <f>IF(upper!E16="", "", upper!E16)</f>
         <v/>
       </c>
-      <c r="F39" s="59" t="str">
+      <c r="F39" s="58" t="str">
         <f>IF(upper!F16=0, "", upper!F16)</f>
         <v/>
       </c>
-      <c r="G39" s="59" t="str">
+      <c r="G39" s="58" t="str">
         <f>IF(upper!A16=0, "", upper!G16)</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="59" t="str">
+      <c r="A40" s="58" t="str">
         <f>IF(upper!A17=0, "", upper!A17)</f>
         <v>triangle_10pad</v>
       </c>
-      <c r="B40" s="59">
+      <c r="B40" s="58">
         <f>IF(upper!B17="", "", upper!B17)</f>
         <v>19</v>
       </c>
-      <c r="C40" s="65">
+      <c r="C40" s="64">
         <f>IF(upper!C17="", "", upper!C17)</f>
         <v>192.37604307033999</v>
       </c>
-      <c r="D40" s="65">
+      <c r="D40" s="64">
         <f>IF(upper!D17="", "", upper!D17)</f>
         <v>-99.999999999999986</v>
       </c>
-      <c r="E40" s="65">
+      <c r="E40" s="64">
         <f>IF(upper!E17="", "", upper!E17)</f>
         <v>-30.000140305771573</v>
       </c>
-      <c r="F40" s="59">
+      <c r="F40" s="58">
         <f>IF(upper!F17=0, "", upper!F17)</f>
         <v>5</v>
       </c>
-      <c r="G40" s="59">
+      <c r="G40" s="58">
         <f>IF(upper!A17=0, "", upper!G17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="59" t="str">
+      <c r="A41" s="58" t="str">
         <f>IF(upper!A18=0, "", upper!A18)</f>
         <v/>
       </c>
-      <c r="B41" s="59" t="str">
+      <c r="B41" s="58" t="str">
         <f>IF(upper!B18="", "", upper!B18)</f>
         <v/>
       </c>
-      <c r="C41" s="65" t="str">
+      <c r="C41" s="64" t="str">
         <f>IF(upper!C18="", "", upper!C18)</f>
         <v/>
       </c>
-      <c r="D41" s="65" t="str">
+      <c r="D41" s="64" t="str">
         <f>IF(upper!D18="", "", upper!D18)</f>
         <v/>
       </c>
-      <c r="E41" s="65" t="str">
+      <c r="E41" s="64" t="str">
         <f>IF(upper!E18="", "", upper!E18)</f>
         <v/>
       </c>
-      <c r="F41" s="59" t="str">
+      <c r="F41" s="58" t="str">
         <f>IF(upper!F18=0, "", upper!F18)</f>
         <v/>
       </c>
-      <c r="G41" s="59" t="str">
+      <c r="G41" s="58" t="str">
         <f>IF(upper!A18=0, "", upper!G18)</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="59" t="str">
+      <c r="A42" s="58" t="str">
         <f>IF(upper!A19=0, "", upper!A19)</f>
         <v/>
       </c>
-      <c r="B42" s="59" t="str">
+      <c r="B42" s="58" t="str">
         <f>IF(upper!B19="", "", upper!B19)</f>
         <v/>
       </c>
-      <c r="C42" s="65" t="str">
+      <c r="C42" s="64" t="str">
         <f>IF(upper!C19="", "", upper!C19)</f>
         <v/>
       </c>
-      <c r="D42" s="65" t="str">
+      <c r="D42" s="64" t="str">
         <f>IF(upper!D19="", "", upper!D19)</f>
         <v/>
       </c>
-      <c r="E42" s="65" t="str">
+      <c r="E42" s="64" t="str">
         <f>IF(upper!E19="", "", upper!E19)</f>
         <v/>
       </c>
-      <c r="F42" s="59" t="str">
+      <c r="F42" s="58" t="str">
         <f>IF(upper!F19=0, "", upper!F19)</f>
         <v/>
       </c>
-      <c r="G42" s="59" t="str">
+      <c r="G42" s="58" t="str">
         <f>IF(upper!A19=0, "", upper!G19)</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="59" t="str">
+      <c r="A43" s="58" t="str">
         <f>IF(upper!A20=0, "", upper!A20)</f>
         <v/>
       </c>
-      <c r="B43" s="59" t="str">
+      <c r="B43" s="58" t="str">
         <f>IF(upper!B20="", "", upper!B20)</f>
         <v/>
       </c>
-      <c r="C43" s="65" t="str">
+      <c r="C43" s="64" t="str">
         <f>IF(upper!C20="", "", upper!C20)</f>
         <v/>
       </c>
-      <c r="D43" s="65" t="str">
+      <c r="D43" s="64" t="str">
         <f>IF(upper!D20="", "", upper!D20)</f>
         <v/>
       </c>
-      <c r="E43" s="65" t="str">
+      <c r="E43" s="64" t="str">
         <f>IF(upper!E20="", "", upper!E20)</f>
         <v/>
       </c>
-      <c r="F43" s="59" t="str">
+      <c r="F43" s="58" t="str">
         <f>IF(upper!F20=0, "", upper!F20)</f>
         <v/>
       </c>
-      <c r="G43" s="59" t="str">
+      <c r="G43" s="58" t="str">
         <f>IF(upper!A20=0, "", upper!G20)</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="59" t="str">
+      <c r="A44" s="58" t="str">
         <f>IF(upper!A21=0, "", upper!A21)</f>
         <v/>
       </c>
-      <c r="B44" s="59" t="str">
+      <c r="B44" s="58" t="str">
         <f>IF(upper!B21="", "", upper!B21)</f>
         <v/>
       </c>
-      <c r="C44" s="65" t="str">
+      <c r="C44" s="64" t="str">
         <f>IF(upper!C21="", "", upper!C21)</f>
         <v/>
       </c>
-      <c r="D44" s="65" t="str">
+      <c r="D44" s="64" t="str">
         <f>IF(upper!D21="", "", upper!D21)</f>
         <v/>
       </c>
-      <c r="E44" s="65" t="str">
+      <c r="E44" s="64" t="str">
         <f>IF(upper!E21="", "", upper!E21)</f>
         <v/>
       </c>
-      <c r="F44" s="59" t="str">
+      <c r="F44" s="58" t="str">
         <f>IF(upper!F21=0, "", upper!F21)</f>
         <v/>
       </c>
-      <c r="G44" s="59" t="str">
+      <c r="G44" s="58" t="str">
         <f>IF(upper!A21=0, "", upper!G21)</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="59" t="str">
+      <c r="A45" s="58" t="str">
         <f>IF(upper!A22=0, "", upper!A22)</f>
         <v/>
       </c>
-      <c r="B45" s="59" t="str">
+      <c r="B45" s="58" t="str">
         <f>IF(upper!B22="", "", upper!B22)</f>
         <v/>
       </c>
-      <c r="C45" s="65" t="str">
+      <c r="C45" s="64" t="str">
         <f>IF(upper!C22="", "", upper!C22)</f>
         <v/>
       </c>
-      <c r="D45" s="65" t="str">
+      <c r="D45" s="64" t="str">
         <f>IF(upper!D22="", "", upper!D22)</f>
         <v/>
       </c>
-      <c r="E45" s="65" t="str">
+      <c r="E45" s="64" t="str">
         <f>IF(upper!E22="", "", upper!E22)</f>
         <v/>
       </c>
-      <c r="F45" s="59" t="str">
+      <c r="F45" s="58" t="str">
         <f>IF(upper!F22=0, "", upper!F22)</f>
         <v/>
       </c>
-      <c r="G45" s="59" t="str">
+      <c r="G45" s="58" t="str">
         <f>IF(upper!A22=0, "", upper!G22)</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="59" t="str">
+      <c r="A46" s="58" t="str">
         <f>IF(upper!A23=0, "", upper!A23)</f>
         <v/>
       </c>
-      <c r="B46" s="59" t="str">
+      <c r="B46" s="58" t="str">
         <f>IF(upper!B23="", "", upper!B23)</f>
         <v/>
       </c>
-      <c r="C46" s="65" t="str">
+      <c r="C46" s="64" t="str">
         <f>IF(upper!C23="", "", upper!C23)</f>
         <v/>
       </c>
-      <c r="D46" s="65" t="str">
+      <c r="D46" s="64" t="str">
         <f>IF(upper!D23="", "", upper!D23)</f>
         <v/>
       </c>
-      <c r="E46" s="65" t="str">
+      <c r="E46" s="64" t="str">
         <f>IF(upper!E23="", "", upper!E23)</f>
         <v/>
       </c>
-      <c r="F46" s="59" t="str">
+      <c r="F46" s="58" t="str">
         <f>IF(upper!F23=0, "", upper!F23)</f>
         <v/>
       </c>
-      <c r="G46" s="59" t="str">
+      <c r="G46" s="58" t="str">
         <f>IF(upper!A23=0, "", upper!G23)</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="59" t="str">
+      <c r="A47" s="58" t="str">
         <f>IF(upper!A24=0, "", upper!A24)</f>
         <v/>
       </c>
-      <c r="B47" s="59" t="str">
+      <c r="B47" s="58" t="str">
         <f>IF(upper!B24="", "", upper!B24)</f>
         <v/>
       </c>
-      <c r="C47" s="65" t="str">
+      <c r="C47" s="64" t="str">
         <f>IF(upper!C24="", "", upper!C24)</f>
         <v/>
       </c>
-      <c r="D47" s="65" t="str">
+      <c r="D47" s="64" t="str">
         <f>IF(upper!D24="", "", upper!D24)</f>
         <v/>
       </c>
-      <c r="E47" s="65" t="str">
+      <c r="E47" s="64" t="str">
         <f>IF(upper!E24="", "", upper!E24)</f>
         <v/>
       </c>
-      <c r="F47" s="59" t="str">
+      <c r="F47" s="58" t="str">
         <f>IF(upper!F24=0, "", upper!F24)</f>
         <v/>
       </c>
-      <c r="G47" s="59" t="str">
+      <c r="G47" s="58" t="str">
         <f>IF(upper!A24=0, "", upper!G24)</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="59" t="str">
+      <c r="A48" s="58" t="str">
         <f>IF(upper!A25=0, "", upper!A25)</f>
         <v/>
       </c>
-      <c r="B48" s="59" t="str">
+      <c r="B48" s="58" t="str">
         <f>IF(upper!B25=0, "", upper!B25)</f>
         <v/>
       </c>
-      <c r="C48" s="65" t="str">
+      <c r="C48" s="64" t="str">
         <f>IF(upper!C25="", "", upper!C25)</f>
         <v/>
       </c>
-      <c r="D48" s="65" t="str">
+      <c r="D48" s="64" t="str">
         <f>IF(upper!D25="", "", upper!D25)</f>
         <v/>
       </c>
-      <c r="E48" s="65" t="str">
+      <c r="E48" s="64" t="str">
         <f>IF(upper!E25="", "", upper!E25)</f>
         <v/>
       </c>
-      <c r="F48" s="59" t="str">
+      <c r="F48" s="58" t="str">
         <f>IF(upper!F25=0, "", upper!F25)</f>
         <v/>
       </c>
-      <c r="G48" s="59" t="str">
+      <c r="G48" s="58" t="str">
         <f>IF(upper!A25=0, "", upper!G25)</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="60"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="66"/>
-      <c r="E49" s="66"/>
-      <c r="F49" s="60"/>
-      <c r="G49" s="60"/>
+      <c r="A49" s="59"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added the triangle number to be put in the xml files
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/forearm_ini_generator iCubV2.xlsx
+++ b/app/skinGui/iniGenerators/forearm_ini_generator iCubV2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12975" activeTab="2"/>
+    <workbookView xWindow="5790" yWindow="-135" windowWidth="12600" windowHeight="12975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="lower" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="30">
   <si>
     <t>[SENSORS]</t>
   </si>
@@ -104,6 +104,9 @@
   <si>
     <t>triangle_10pad_10pad #</t>
   </si>
+  <si>
+    <t>Triangle # for the MTB</t>
+  </si>
 </sst>
 </file>
 
@@ -173,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +260,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,7 +641,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -758,6 +773,11 @@
     <xf numFmtId="2" fontId="6" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -785,13 +805,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>534787</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>150712</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>897673</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>46190</xdr:rowOff>
@@ -803,7 +823,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10069312" y="2417662"/>
+          <a:off x="10707487" y="2417662"/>
           <a:ext cx="4353861" cy="4096003"/>
           <a:chOff x="10968014" y="1847464"/>
           <a:chExt cx="5518210" cy="4625913"/>
@@ -1809,13 +1829,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>2505075</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -1968,13 +1988,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>5620</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1681</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1986,7 +2006,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10641870" y="0"/>
+          <a:off x="11276870" y="0"/>
           <a:ext cx="4038894" cy="0"/>
           <a:chOff x="10981462" y="1799664"/>
           <a:chExt cx="5588677" cy="4621561"/>
@@ -2992,13 +3012,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>534787</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>150712</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>46190</xdr:rowOff>
@@ -3010,7 +3030,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10599537" y="2320295"/>
+          <a:off x="11234537" y="2320295"/>
           <a:ext cx="4524046" cy="3716062"/>
           <a:chOff x="10968014" y="1847464"/>
           <a:chExt cx="5518210" cy="4625913"/>
@@ -4016,13 +4036,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>211666</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>148167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>2550583</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>42333</xdr:rowOff>
@@ -4431,10 +4451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4451,23 +4471,24 @@
     <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" customWidth="1"/>
-    <col min="20" max="20" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.42578125" customWidth="1"/>
+    <col min="21" max="21" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -4500,20 +4521,23 @@
       <c r="L2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="O2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="P2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="Q2" s="33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>26</v>
       </c>
@@ -4522,22 +4546,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="23">
-        <f>((+O3*COS($N$3)-P3*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P3*COS($O$3)-Q3*SIN($O$3)+$O$7)*$S$3)</f>
         <v>100</v>
       </c>
       <c r="D3" s="23">
-        <f>((O3*SIN($N$3)+P3*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P3*SIN($O$3)+Q3*COS($O$3)+$O$9)*$S$4)</f>
         <v>-20</v>
       </c>
       <c r="E3" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N3/3.1416*180)+$O$5)</f>
         <v>29.999719388456853</v>
       </c>
       <c r="F3" s="11">
         <v>5</v>
       </c>
       <c r="G3" s="25">
-        <f t="shared" ref="G3:G5" si="1">IF($R$3*$R$4=-1,1,0)</f>
+        <f t="shared" ref="G3:G5" si="1">IF($S$3*$S$4=-1,1,0)</f>
         <v>1</v>
       </c>
       <c r="H3" s="1"/>
@@ -4551,30 +4575,34 @@
       <c r="L3" s="13">
         <v>10</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="69">
+        <f>(ROUND((L3/10),0)-1)*4+(MOD(L3,10))</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
         <v>-2.0943951023932001</v>
       </c>
-      <c r="N3" s="14">
-        <f>+RADIANS(N5)</f>
+      <c r="O3" s="14">
+        <f>+RADIANS(O5)</f>
         <v>1.5707963267948966</v>
       </c>
-      <c r="O3" s="15">
+      <c r="P3" s="15">
         <v>100</v>
       </c>
-      <c r="P3" s="40">
+      <c r="Q3" s="40">
         <v>100</v>
       </c>
-      <c r="Q3" s="51" t="s">
+      <c r="R3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="52">
+      <c r="S3" s="52">
         <v>-1</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="U3" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>26</v>
       </c>
@@ -4583,15 +4611,15 @@
         <v>1</v>
       </c>
       <c r="C4" s="23">
-        <f>((+O4*COS($N$3)-P4*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P4*COS($O$3)-Q4*SIN($O$3)+$O$7)*$S$3)</f>
         <v>109.23760430703399</v>
       </c>
       <c r="D4" s="23">
-        <f>((O4*SIN($N$3)+P4*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P4*SIN($O$3)+Q4*COS($O$3)+$O$9)*$S$4)</f>
         <v>-4</v>
       </c>
       <c r="E4" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M4/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N4/3.1416*180)+$O$5)</f>
         <v>-30.000140305771573</v>
       </c>
       <c r="F4" s="11">
@@ -4612,27 +4640,31 @@
       <c r="L4" s="5">
         <v>11</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="69">
+        <f t="shared" ref="M4:M25" si="2">(ROUND((L4/10),0)-1)*4+(MOD(L4,10))</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="42">
+      <c r="P4" s="42">
         <v>116</v>
       </c>
-      <c r="P4" s="43">
+      <c r="Q4" s="43">
         <v>109.237604307034</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="R4" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="54">
+      <c r="S4" s="54">
         <v>1</v>
       </c>
-      <c r="S4" s="9"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T4" s="9"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>26</v>
       </c>
@@ -4641,15 +4673,15 @@
         <v>2</v>
       </c>
       <c r="C5" s="23">
-        <f>((+O5*COS($N$3)-P5*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P5*COS($O$3)-Q5*SIN($O$3)+$O$7)*$S$3)</f>
         <v>99.999999999999986</v>
       </c>
       <c r="D5" s="23">
-        <f>((O5*SIN($N$3)+P5*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P5*SIN($O$3)+Q5*COS($O$3)+$O$9)*$S$4)</f>
         <v>12</v>
       </c>
       <c r="E5" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M5/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N5/3.1416*180)+$O$5)</f>
         <v>29.999719388456853</v>
       </c>
       <c r="F5" s="11">
@@ -4670,26 +4702,30 @@
       <c r="L5" s="5">
         <v>12</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="69">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N5" s="6">
         <v>-2.0943951023932001</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>90</v>
       </c>
-      <c r="O5" s="42">
+      <c r="P5" s="42">
         <v>132</v>
       </c>
-      <c r="P5" s="43">
+      <c r="Q5" s="43">
         <v>100</v>
       </c>
-      <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-      <c r="T5" s="16" t="s">
+      <c r="T5" s="9"/>
+      <c r="U5" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="34"/>
       <c r="C6" s="23"/>
@@ -4708,24 +4744,28 @@
       <c r="L6" s="5">
         <v>13</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="68">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N6" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N6" s="44" t="s">
+      <c r="O6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="42">
+      <c r="P6" s="42">
         <v>148</v>
       </c>
-      <c r="P6" s="43">
+      <c r="Q6" s="43">
         <v>109.237604307034</v>
       </c>
-      <c r="S6" s="9"/>
-      <c r="T6" s="17" t="s">
+      <c r="T6" s="9"/>
+      <c r="U6" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24"/>
       <c r="B7" s="34"/>
       <c r="C7" s="23"/>
@@ -4744,23 +4784,27 @@
       <c r="L7" s="5">
         <v>20</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="68">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N7" s="6">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>0</v>
       </c>
-      <c r="O7" s="42">
+      <c r="P7" s="42">
         <v>148</v>
       </c>
-      <c r="P7" s="43">
+      <c r="Q7" s="43">
         <v>127.712812921102</v>
       </c>
-      <c r="T7" s="18" t="s">
+      <c r="U7" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24"/>
       <c r="B8" s="34"/>
       <c r="C8" s="23"/>
@@ -4779,23 +4823,27 @@
       <c r="L8" s="5">
         <v>21</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="68">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N8" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N8" s="44" t="s">
+      <c r="O8" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="42">
+      <c r="P8" s="42">
         <v>164</v>
       </c>
-      <c r="P8" s="43">
+      <c r="Q8" s="43">
         <v>136.95041722813599</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="U8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="34"/>
       <c r="C9" s="23"/>
@@ -4813,21 +4861,25 @@
       <c r="L9" s="5">
         <v>22</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="68">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N9" s="6">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="3">
         <v>-120</v>
       </c>
-      <c r="O9" s="42">
+      <c r="P9" s="42">
         <v>164</v>
       </c>
-      <c r="P9" s="43">
+      <c r="Q9" s="43">
         <v>155.425625842204</v>
       </c>
-      <c r="T9" s="7"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="34"/>
       <c r="C10" s="23"/>
@@ -4845,44 +4897,48 @@
       <c r="L10" s="5">
         <v>23</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="68">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N10" s="6">
         <v>1.0471975511966001</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="42">
+      <c r="P10" s="42">
         <v>148</v>
       </c>
-      <c r="P10" s="43">
+      <c r="Q10" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="23">
-        <f t="shared" ref="B11:B20" si="2">((ROUND($L11/10,0))-1)*4+MOD($L11,10)+((J11-1)*16)</f>
+        <f t="shared" ref="B11:B20" si="3">((ROUND($L11/10,0))-1)*4+MOD($L11,10)+((J11-1)*16)</f>
         <v>12</v>
       </c>
       <c r="C11" s="23">
-        <f t="shared" ref="C11:C20" si="3">((+O11*COS($N$3)-P11*SIN($N$3)+$N$7)*$R$3)</f>
+        <f t="shared" ref="C11:C20" si="4">((+P11*COS($O$3)-Q11*SIN($O$3)+$O$7)*$S$3)</f>
         <v>127.712812921102</v>
       </c>
       <c r="D11" s="23">
-        <f t="shared" ref="D11:D20" si="4">((O11*SIN($N$3)+P11*COS($N$3)+$N$9)*$R$4)</f>
+        <f t="shared" ref="D11:D20" si="5">((P11*SIN($O$3)+Q11*COS($O$3)+$O$9)*$S$4)</f>
         <v>-3.9999999999999858</v>
       </c>
       <c r="E11" s="23">
-        <f t="shared" ref="E11:E20" si="5">IF(($R$3*$R$4)=1,1,-1)*(($M11/3.1416*180)+$N$5)</f>
+        <f t="shared" ref="E11:E20" si="6">IF(($S$3*$S$4)=1,1,-1)*(($N11/3.1416*180)+$O$5)</f>
         <v>-90</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
       </c>
       <c r="G11" s="25">
-        <f t="shared" ref="G11:G20" si="6">IF($R$3*$R$4=-1,1,0)</f>
+        <f t="shared" ref="G11:G20" si="7">IF($S$3*$S$4=-1,1,0)</f>
         <v>1</v>
       </c>
       <c r="I11" s="1"/>
@@ -4895,44 +4951,48 @@
       <c r="L11" s="5">
         <v>40</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="69">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N11" s="6">
         <v>0</v>
       </c>
-      <c r="N11" s="56">
+      <c r="O11" s="56">
         <v>0</v>
       </c>
-      <c r="O11" s="42">
+      <c r="P11" s="42">
         <v>116</v>
       </c>
-      <c r="P11" s="43">
+      <c r="Q11" s="43">
         <v>127.712812921102</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="C12" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>136.95041722813599</v>
       </c>
       <c r="D12" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="E12" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-30.000140305771573</v>
       </c>
       <c r="F12" s="11">
         <v>5</v>
       </c>
       <c r="G12" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I12" s="1"/>
@@ -4945,42 +5005,46 @@
       <c r="L12" s="5">
         <v>41</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="69">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N12" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="42">
+      <c r="O12" s="4"/>
+      <c r="P12" s="42">
         <v>132</v>
       </c>
-      <c r="P12" s="43">
+      <c r="Q12" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="C13" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>155.425625842204</v>
       </c>
       <c r="D13" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="E13" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-90</v>
       </c>
       <c r="F13" s="11">
         <v>5</v>
       </c>
       <c r="G13" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I13" s="1"/>
@@ -4993,42 +5057,46 @@
       <c r="L13" s="5">
         <v>30</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="69">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N13" s="6">
         <v>0</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="42">
+      <c r="O13" s="4"/>
+      <c r="P13" s="42">
         <v>132</v>
       </c>
-      <c r="P13" s="43">
+      <c r="Q13" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="C14" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>164.66323014923799</v>
       </c>
       <c r="D14" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.9999999999999858</v>
       </c>
       <c r="E14" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-149.99985969422843</v>
       </c>
       <c r="F14" s="11">
         <v>5</v>
       </c>
       <c r="G14" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I14" s="1"/>
@@ -5041,42 +5109,46 @@
       <c r="L14" s="5">
         <v>31</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="69">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N14" s="6">
         <v>1.0471975511966001</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="42">
+      <c r="O14" s="4"/>
+      <c r="P14" s="42">
         <v>116</v>
       </c>
-      <c r="P14" s="43">
+      <c r="Q14" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="C15" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>183.138438763306</v>
       </c>
       <c r="D15" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.9999999999999858</v>
       </c>
       <c r="E15" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-90</v>
       </c>
       <c r="F15" s="11">
         <v>5</v>
       </c>
       <c r="G15" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I15" s="1"/>
@@ -5089,42 +5161,46 @@
       <c r="L15" s="5">
         <v>22</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="69">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N15" s="6">
         <v>0</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="42">
+      <c r="O15" s="4"/>
+      <c r="P15" s="42">
         <v>116</v>
       </c>
-      <c r="P15" s="43">
+      <c r="Q15" s="43">
         <v>183.138438763306</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="C16" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>192.37604307033999</v>
       </c>
       <c r="D16" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="E16" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-30.000140305771573</v>
       </c>
       <c r="F16" s="11">
         <v>5</v>
       </c>
       <c r="G16" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I16" s="1"/>
@@ -5137,42 +5213,46 @@
       <c r="L16" s="5">
         <v>23</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="69">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N16" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="42">
+      <c r="O16" s="4"/>
+      <c r="P16" s="42">
         <v>132</v>
       </c>
-      <c r="P16" s="43">
+      <c r="Q16" s="43">
         <v>192.37604307033999</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="C17" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>192.37604307033999</v>
       </c>
       <c r="D17" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-19.999999999999986</v>
       </c>
       <c r="E17" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-149.99985969422843</v>
       </c>
       <c r="F17" s="11">
         <v>5</v>
       </c>
       <c r="G17" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I17" s="1"/>
@@ -5185,42 +5265,46 @@
       <c r="L17" s="5">
         <v>13</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="69">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N17" s="6">
         <v>1.0471975511966001</v>
       </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="42">
+      <c r="O17" s="4"/>
+      <c r="P17" s="42">
         <v>100</v>
       </c>
-      <c r="P17" s="43">
+      <c r="Q17" s="43">
         <v>192.37604307033999</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="C18" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>183.138438763306</v>
       </c>
       <c r="D18" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-35.999999999999986</v>
       </c>
       <c r="E18" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-209.99971938845687</v>
       </c>
       <c r="F18" s="11">
         <v>5</v>
       </c>
       <c r="G18" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I18" s="1"/>
@@ -5233,42 +5317,46 @@
       <c r="L18" s="5">
         <v>20</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="69">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N18" s="6">
         <v>2.0943951023932001</v>
       </c>
-      <c r="N18" s="4"/>
-      <c r="O18" s="42">
+      <c r="O18" s="4"/>
+      <c r="P18" s="42">
         <v>84</v>
       </c>
-      <c r="P18" s="43">
+      <c r="Q18" s="43">
         <v>183.138438763306</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="C19" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>155.425625842204</v>
       </c>
       <c r="D19" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-19.999999999999986</v>
       </c>
       <c r="E19" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-209.99971938845687</v>
       </c>
       <c r="F19" s="11">
         <v>5</v>
       </c>
       <c r="G19" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I19" s="1"/>
@@ -5281,42 +5369,46 @@
       <c r="L19" s="5">
         <v>32</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="69">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N19" s="6">
         <v>2.0943951023932001</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="42">
+      <c r="O19" s="4"/>
+      <c r="P19" s="42">
         <v>100</v>
       </c>
-      <c r="P19" s="43">
+      <c r="Q19" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="C20" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>164.66323014923799</v>
       </c>
       <c r="D20" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-35.999999999999986</v>
       </c>
       <c r="E20" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-149.99985969422843</v>
       </c>
       <c r="F20" s="11">
         <v>5</v>
       </c>
       <c r="G20" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I20" s="2"/>
@@ -5329,18 +5421,22 @@
       <c r="L20" s="5">
         <v>21</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="68">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N20" s="6">
         <v>1.0471975511966001</v>
       </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="42">
+      <c r="O20" s="4"/>
+      <c r="P20" s="42">
         <v>84</v>
       </c>
-      <c r="P20" s="43">
+      <c r="Q20" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="34"/>
       <c r="C21" s="23"/>
@@ -5358,18 +5454,22 @@
       <c r="L21" s="5">
         <v>43</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="68">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N21" s="6">
         <v>2.0943951023932001</v>
       </c>
-      <c r="N21" s="4"/>
-      <c r="O21" s="42">
+      <c r="O21" s="4"/>
+      <c r="P21" s="42">
         <v>68</v>
       </c>
-      <c r="P21" s="43">
+      <c r="Q21" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="34"/>
       <c r="C22" s="23"/>
@@ -5387,42 +5487,46 @@
       <c r="L22" s="5">
         <v>10</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="68">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="6">
         <v>3.14159265358979</v>
       </c>
-      <c r="N22" s="4"/>
-      <c r="O22" s="42">
+      <c r="O22" s="4"/>
+      <c r="P22" s="42">
         <v>68</v>
       </c>
-      <c r="P22" s="43">
+      <c r="Q22" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="23">
-        <f t="shared" ref="B23:B25" si="7">((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
+        <f t="shared" ref="B23:B25" si="8">((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
         <v>11</v>
       </c>
       <c r="C23" s="23">
-        <f>((+O23*COS($N$3)-P23*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P23*COS($O$3)-Q23*SIN($O$3)+$O$7)*$S$3)</f>
         <v>136.95041722813599</v>
       </c>
       <c r="D23" s="23">
-        <f>((O23*SIN($N$3)+P23*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P23*SIN($O$3)+Q23*COS($O$3)+$O$9)*$S$4)</f>
         <v>-19.999999999999986</v>
       </c>
       <c r="E23" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M23/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N23/3.1416*180)+$O$5)</f>
         <v>-269.9995790826847</v>
       </c>
       <c r="F23" s="11">
         <v>5</v>
       </c>
       <c r="G23" s="25">
-        <f t="shared" ref="G23:G25" si="8">IF($R$3*$R$4=-1,1,0)</f>
+        <f t="shared" ref="G23:G25" si="9">IF($S$3*$S$4=-1,1,0)</f>
         <v>1</v>
       </c>
       <c r="I23" s="2"/>
@@ -5435,42 +5539,46 @@
       <c r="L23" s="5">
         <v>33</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="69">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N23" s="6">
         <v>3.14159265358979</v>
       </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="42">
+      <c r="O23" s="4"/>
+      <c r="P23" s="42">
         <v>100</v>
       </c>
-      <c r="P23" s="43">
+      <c r="Q23" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="C24" s="23">
-        <f>((+O24*COS($N$3)-P24*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P24*COS($O$3)-Q24*SIN($O$3)+$O$7)*$S$3)</f>
         <v>127.712812921102</v>
       </c>
       <c r="D24" s="23">
-        <f>((O24*SIN($N$3)+P24*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P24*SIN($O$3)+Q24*COS($O$3)+$O$9)*$S$4)</f>
         <v>-35.999999999999986</v>
       </c>
       <c r="E24" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M24/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N24/3.1416*180)+$O$5)</f>
         <v>-209.99971938845687</v>
       </c>
       <c r="F24" s="11">
         <v>5</v>
       </c>
       <c r="G24" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I24" s="2"/>
@@ -5483,42 +5591,46 @@
       <c r="L24" s="5">
         <v>42</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M24" s="69">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="N24" s="6">
         <v>2.0943951023932001</v>
       </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="42">
+      <c r="O24" s="4"/>
+      <c r="P24" s="42">
         <v>84</v>
       </c>
-      <c r="P24" s="43">
+      <c r="Q24" s="43">
         <v>127.712812921102</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="C25" s="23">
-        <f>((+O25*COS($N$3)-P25*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P25*COS($O$3)-Q25*SIN($O$3)+$O$7)*$S$3)</f>
         <v>109.237604307034</v>
       </c>
       <c r="D25" s="23">
-        <f>((O25*SIN($N$3)+P25*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P25*SIN($O$3)+Q25*COS($O$3)+$O$9)*$S$4)</f>
         <v>-36</v>
       </c>
       <c r="E25" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M25/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N25/3.1416*180)+$O$5)</f>
         <v>-269.9995790826847</v>
       </c>
       <c r="F25" s="11">
         <v>5</v>
       </c>
       <c r="G25" s="25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I25" s="2"/>
@@ -5531,260 +5643,288 @@
       <c r="L25" s="46">
         <v>43</v>
       </c>
-      <c r="M25" s="47">
+      <c r="M25" s="69">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N25" s="47">
         <v>3.14159265358979</v>
       </c>
-      <c r="N25" s="48"/>
-      <c r="O25" s="49">
+      <c r="O25" s="48"/>
+      <c r="P25" s="49">
         <v>84</v>
       </c>
-      <c r="P25" s="50">
+      <c r="Q25" s="50">
         <v>109.237604307034</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N31" s="7"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G32" s="7"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="7"/>
-    </row>
-    <row r="33" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="M32" s="8"/>
+      <c r="N32" s="7"/>
+    </row>
+    <row r="33" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G33" s="7"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
-      <c r="M33" s="7"/>
+      <c r="M33" s="8"/>
       <c r="N33" s="7"/>
-    </row>
-    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G34" s="7"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
-      <c r="M34" s="7"/>
+      <c r="M34" s="8"/>
       <c r="N34" s="7"/>
-    </row>
-    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G35" s="7"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
-      <c r="M35" s="7"/>
+      <c r="M35" s="8"/>
       <c r="N35" s="7"/>
-    </row>
-    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G36" s="7"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
-      <c r="M36" s="7"/>
+      <c r="M36" s="8"/>
       <c r="N36" s="7"/>
-    </row>
-    <row r="37" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G37" s="7"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
-      <c r="M37" s="7"/>
+      <c r="M37" s="8"/>
       <c r="N37" s="7"/>
-    </row>
-    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G38" s="7"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
-      <c r="M38" s="7"/>
+      <c r="M38" s="8"/>
       <c r="N38" s="7"/>
-    </row>
-    <row r="39" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G39" s="7"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
-      <c r="M39" s="7"/>
+      <c r="M39" s="8"/>
       <c r="N39" s="7"/>
-    </row>
-    <row r="40" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="7"/>
+    </row>
+    <row r="40" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G40" s="7"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
-      <c r="M40" s="7"/>
+      <c r="M40" s="8"/>
       <c r="N40" s="7"/>
-    </row>
-    <row r="41" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G41" s="7"/>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
-      <c r="M41" s="7"/>
+      <c r="M41" s="8"/>
       <c r="N41" s="7"/>
-    </row>
-    <row r="42" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="7"/>
+    </row>
+    <row r="42" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G42" s="7"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
-      <c r="M42" s="7"/>
+      <c r="M42" s="8"/>
       <c r="N42" s="7"/>
-    </row>
-    <row r="43" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="7"/>
+    </row>
+    <row r="43" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G43" s="7"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
-      <c r="M43" s="7"/>
+      <c r="M43" s="8"/>
       <c r="N43" s="7"/>
-    </row>
-    <row r="44" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="7"/>
+    </row>
+    <row r="44" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G44" s="7"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
-      <c r="M44" s="7"/>
+      <c r="M44" s="8"/>
       <c r="N44" s="7"/>
-    </row>
-    <row r="45" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G45" s="7"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
-      <c r="M45" s="7"/>
+      <c r="M45" s="8"/>
       <c r="N45" s="7"/>
-    </row>
-    <row r="46" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O45" s="7"/>
+    </row>
+    <row r="46" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G46" s="7"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
-      <c r="M46" s="7"/>
+      <c r="M46" s="8"/>
       <c r="N46" s="7"/>
-    </row>
-    <row r="47" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="7"/>
+    </row>
+    <row r="47" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G47" s="7"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
-      <c r="M47" s="7"/>
+      <c r="M47" s="8"/>
       <c r="N47" s="7"/>
-    </row>
-    <row r="48" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="7"/>
+    </row>
+    <row r="48" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G48" s="7"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
-      <c r="M48" s="7"/>
+      <c r="M48" s="8"/>
       <c r="N48" s="7"/>
-    </row>
-    <row r="49" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O48" s="7"/>
+    </row>
+    <row r="49" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G49" s="7"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
-      <c r="M49" s="7"/>
+      <c r="M49" s="8"/>
       <c r="N49" s="7"/>
-    </row>
-    <row r="50" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="7"/>
+    </row>
+    <row r="50" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G50" s="7"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
-      <c r="M50" s="7"/>
+      <c r="M50" s="8"/>
       <c r="N50" s="7"/>
-    </row>
-    <row r="51" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="7"/>
+    </row>
+    <row r="51" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G51" s="7"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
-      <c r="M51" s="7"/>
+      <c r="M51" s="8"/>
       <c r="N51" s="7"/>
-    </row>
-    <row r="52" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="7"/>
+    </row>
+    <row r="52" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G52" s="7"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
-      <c r="M52" s="7"/>
+      <c r="M52" s="8"/>
       <c r="N52" s="7"/>
-    </row>
-    <row r="53" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O52" s="7"/>
+    </row>
+    <row r="53" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G53" s="7"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
-      <c r="M53" s="7"/>
+      <c r="M53" s="8"/>
       <c r="N53" s="7"/>
-    </row>
-    <row r="54" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O53" s="7"/>
+    </row>
+    <row r="54" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G54" s="7"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
-      <c r="M54" s="7"/>
+      <c r="M54" s="8"/>
       <c r="N54" s="7"/>
-    </row>
-    <row r="55" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="O54" s="7"/>
+    </row>
+    <row r="55" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
@@ -5793,6 +5933,7 @@
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5803,10 +5944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5818,20 +5959,21 @@
     <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -5864,20 +6006,23 @@
       <c r="L2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="O2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="P2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="Q2" s="33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>26</v>
       </c>
@@ -5886,22 +6031,22 @@
         <v>16</v>
       </c>
       <c r="C3" s="23">
-        <f>((+O3*COS($N$3)-P3*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P3*COS($O$3)-Q3*SIN($O$3)+$O$7)*$S$3)</f>
         <v>100</v>
       </c>
       <c r="D3" s="23">
-        <f>((O3*SIN($N$3)+P3*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P3*SIN($O$3)+Q3*COS($O$3)+$O$9)*$S$4)</f>
         <v>-100</v>
       </c>
       <c r="E3" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M3/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N3/3.1416*180)+$O$5)</f>
         <v>-209.99971938845687</v>
       </c>
       <c r="F3" s="11">
         <v>5</v>
       </c>
       <c r="G3" s="25">
-        <f t="shared" ref="G3:G4" si="1">IF($R$3*$R$4=-1,1,0)</f>
+        <f t="shared" ref="G3:G4" si="1">IF($S$3*$S$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="H3" s="1"/>
@@ -5915,30 +6060,34 @@
       <c r="L3" s="13">
         <v>10</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="69">
+        <f>(ROUND((L3/10),0)-1)*4+(MOD(L3,10))</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
         <v>-2.0943951023932001</v>
       </c>
-      <c r="N3" s="14">
-        <f>+RADIANS(N5)</f>
+      <c r="O3" s="14">
+        <f>+RADIANS(O5)</f>
         <v>-1.5707963267948966</v>
       </c>
-      <c r="O3" s="15">
+      <c r="P3" s="15">
         <v>100</v>
       </c>
-      <c r="P3" s="40">
+      <c r="Q3" s="40">
         <v>100</v>
       </c>
-      <c r="Q3" s="51" t="s">
+      <c r="R3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="52">
+      <c r="S3" s="52">
         <v>1</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="U3" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>26</v>
       </c>
@@ -5947,15 +6096,15 @@
         <v>17</v>
       </c>
       <c r="C4" s="23">
-        <f>((+O4*COS($N$3)-P4*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P4*COS($O$3)-Q4*SIN($O$3)+$O$7)*$S$3)</f>
         <v>109.23760430703402</v>
       </c>
       <c r="D4" s="23">
-        <f>((O4*SIN($N$3)+P4*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P4*SIN($O$3)+Q4*COS($O$3)+$O$9)*$S$4)</f>
         <v>-116</v>
       </c>
       <c r="E4" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M4/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N4/3.1416*180)+$O$5)</f>
         <v>-149.99985969422843</v>
       </c>
       <c r="F4" s="11">
@@ -5976,27 +6125,31 @@
       <c r="L4" s="5">
         <v>11</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="69">
+        <f t="shared" ref="M4:M25" si="3">(ROUND((L4/10),0)-1)*4+(MOD(L4,10))</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="42">
+      <c r="P4" s="42">
         <v>116</v>
       </c>
-      <c r="P4" s="43">
+      <c r="Q4" s="43">
         <v>109.237604307034</v>
       </c>
-      <c r="Q4" s="53" t="s">
+      <c r="R4" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="54">
+      <c r="S4" s="54">
         <v>1</v>
       </c>
-      <c r="S4" s="9"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T4" s="9"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="34"/>
       <c r="C5" s="23"/>
@@ -6015,26 +6168,30 @@
       <c r="L5" s="5">
         <v>12</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="68">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="N5" s="6">
         <v>-2.0943951023932001</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>-90</v>
       </c>
-      <c r="O5" s="42">
+      <c r="P5" s="42">
         <v>132</v>
       </c>
-      <c r="P5" s="43">
+      <c r="Q5" s="43">
         <v>100</v>
       </c>
-      <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
-      <c r="T5" s="16" t="s">
+      <c r="T5" s="9"/>
+      <c r="U5" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="34"/>
       <c r="C6" s="23"/>
@@ -6053,24 +6210,28 @@
       <c r="L6" s="5">
         <v>13</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="68">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N6" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N6" s="44" t="s">
+      <c r="O6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="42">
+      <c r="P6" s="42">
         <v>148</v>
       </c>
-      <c r="P6" s="43">
+      <c r="Q6" s="43">
         <v>109.237604307034</v>
       </c>
-      <c r="S6" s="9"/>
-      <c r="T6" s="17" t="s">
+      <c r="T6" s="9"/>
+      <c r="U6" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24"/>
       <c r="B7" s="34"/>
       <c r="C7" s="23"/>
@@ -6089,23 +6250,27 @@
       <c r="L7" s="5">
         <v>20</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="68">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="N7" s="6">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>0</v>
       </c>
-      <c r="O7" s="42">
+      <c r="P7" s="42">
         <v>148</v>
       </c>
-      <c r="P7" s="43">
+      <c r="Q7" s="43">
         <v>127.712812921102</v>
       </c>
-      <c r="T7" s="18" t="s">
+      <c r="U7" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24"/>
       <c r="B8" s="34"/>
       <c r="C8" s="23"/>
@@ -6124,23 +6289,27 @@
       <c r="L8" s="5">
         <v>21</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="68">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="N8" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N8" s="44" t="s">
+      <c r="O8" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="42">
+      <c r="P8" s="42">
         <v>164</v>
       </c>
-      <c r="P8" s="43">
+      <c r="Q8" s="43">
         <v>136.95041722813599</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="U8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="34"/>
       <c r="C9" s="23"/>
@@ -6158,21 +6327,25 @@
       <c r="L9" s="5">
         <v>22</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="68">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N9" s="6">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="3">
         <v>0</v>
       </c>
-      <c r="O9" s="42">
+      <c r="P9" s="42">
         <v>164</v>
       </c>
-      <c r="P9" s="43">
+      <c r="Q9" s="43">
         <v>155.425625842204</v>
       </c>
-      <c r="T9" s="7"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="34"/>
       <c r="C10" s="23"/>
@@ -6190,44 +6363,48 @@
       <c r="L10" s="5">
         <v>23</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="68">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="N10" s="6">
         <v>1.0471975511966001</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="42">
+      <c r="P10" s="42">
         <v>148</v>
       </c>
-      <c r="P10" s="43">
+      <c r="Q10" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="23">
-        <f t="shared" ref="B11:B15" si="3">((ROUND($L11/10,0))-1)*4+MOD($L11,10)+((J11-1)*16)</f>
+        <f t="shared" ref="B11:B15" si="4">((ROUND($L11/10,0))-1)*4+MOD($L11,10)+((J11-1)*16)</f>
         <v>28</v>
       </c>
       <c r="C11" s="23">
-        <f t="shared" ref="C11:C15" si="4">((+O11*COS($N$3)-P11*SIN($N$3)+$N$7)*$R$3)</f>
+        <f t="shared" ref="C11:C15" si="5">((+P11*COS($O$3)-Q11*SIN($O$3)+$O$7)*$S$3)</f>
         <v>127.712812921102</v>
       </c>
       <c r="D11" s="23">
-        <f t="shared" ref="D11:D15" si="5">((O11*SIN($N$3)+P11*COS($N$3)+$N$9)*$R$4)</f>
+        <f t="shared" ref="D11:D15" si="6">((P11*SIN($O$3)+Q11*COS($O$3)+$O$9)*$S$4)</f>
         <v>-115.99999999999999</v>
       </c>
       <c r="E11" s="23">
-        <f t="shared" ref="E11:E15" si="6">IF(($R$3*$R$4)=1,1,-1)*(($M11/3.1416*180)+$N$5)</f>
+        <f t="shared" ref="E11:E15" si="7">IF(($S$3*$S$4)=1,1,-1)*(($N11/3.1416*180)+$O$5)</f>
         <v>-90</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
       </c>
       <c r="G11" s="25">
-        <f t="shared" ref="G11:G15" si="7">IF($R$3*$R$4=-1,1,0)</f>
+        <f t="shared" ref="G11:G15" si="8">IF($S$3*$S$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="I11" s="1"/>
@@ -6240,45 +6417,49 @@
       <c r="L11" s="5">
         <v>40</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="69">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="N11" s="6">
         <v>0</v>
       </c>
-      <c r="N11" s="56">
+      <c r="O11" s="56">
         <f>16*3</f>
         <v>48</v>
       </c>
-      <c r="O11" s="42">
+      <c r="P11" s="42">
         <v>116</v>
       </c>
-      <c r="P11" s="43">
+      <c r="Q11" s="43">
         <v>127.712812921102</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="C12" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>136.95041722813599</v>
       </c>
       <c r="D12" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-132</v>
       </c>
       <c r="E12" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-149.99985969422843</v>
       </c>
       <c r="F12" s="11">
         <v>5</v>
       </c>
       <c r="G12" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I12" s="1"/>
@@ -6291,42 +6472,46 @@
       <c r="L12" s="5">
         <v>41</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="69">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="N12" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="42">
+      <c r="O12" s="4"/>
+      <c r="P12" s="42">
         <v>132</v>
       </c>
-      <c r="P12" s="43">
+      <c r="Q12" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="C13" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>155.425625842204</v>
       </c>
       <c r="D13" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-132</v>
       </c>
       <c r="E13" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-90</v>
       </c>
       <c r="F13" s="11">
         <v>5</v>
       </c>
       <c r="G13" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I13" s="1"/>
@@ -6339,42 +6524,46 @@
       <c r="L13" s="5">
         <v>30</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="69">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="N13" s="6">
         <v>0</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="42">
+      <c r="O13" s="4"/>
+      <c r="P13" s="42">
         <v>132</v>
       </c>
-      <c r="P13" s="43">
+      <c r="Q13" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="C14" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>164.66323014923799</v>
       </c>
       <c r="D14" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-115.99999999999999</v>
       </c>
       <c r="E14" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-30.000140305771573</v>
       </c>
       <c r="F14" s="11">
         <v>5</v>
       </c>
       <c r="G14" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I14" s="1"/>
@@ -6387,42 +6576,46 @@
       <c r="L14" s="5">
         <v>31</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="69">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="N14" s="6">
         <v>1.0471975511966001</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="42">
+      <c r="O14" s="4"/>
+      <c r="P14" s="42">
         <v>116</v>
       </c>
-      <c r="P14" s="43">
+      <c r="Q14" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="C15" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>183.138438763306</v>
       </c>
       <c r="D15" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-115.99999999999999</v>
       </c>
       <c r="E15" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-90</v>
       </c>
       <c r="F15" s="11">
         <v>5</v>
       </c>
       <c r="G15" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I15" s="1"/>
@@ -6435,18 +6628,22 @@
       <c r="L15" s="5">
         <v>22</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="69">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N15" s="6">
         <v>0</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="42">
+      <c r="O15" s="4"/>
+      <c r="P15" s="42">
         <v>116</v>
       </c>
-      <c r="P15" s="43">
+      <c r="Q15" s="43">
         <v>183.138438763306</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="34"/>
       <c r="C16" s="23"/>
@@ -6464,42 +6661,46 @@
       <c r="L16" s="5">
         <v>23</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="68">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="N16" s="6">
         <v>-1.0471975511966001</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="42">
+      <c r="O16" s="4"/>
+      <c r="P16" s="42">
         <v>132</v>
       </c>
-      <c r="P16" s="43">
+      <c r="Q16" s="43">
         <v>192.37604307033999</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="23">
-        <f t="shared" ref="B17" si="8">((ROUND($L17/10,0))-1)*4+MOD($L17,10)+((J17-1)*16)</f>
+        <f t="shared" ref="B17" si="9">((ROUND($L17/10,0))-1)*4+MOD($L17,10)+((J17-1)*16)</f>
         <v>19</v>
       </c>
       <c r="C17" s="23">
-        <f>((+O17*COS($N$3)-P17*SIN($N$3)+$N$7)*$R$3)</f>
+        <f>((+P17*COS($O$3)-Q17*SIN($O$3)+$O$7)*$S$3)</f>
         <v>192.37604307033999</v>
       </c>
       <c r="D17" s="23">
-        <f>((O17*SIN($N$3)+P17*COS($N$3)+$N$9)*$R$4)</f>
+        <f>((P17*SIN($O$3)+Q17*COS($O$3)+$O$9)*$S$4)</f>
         <v>-99.999999999999986</v>
       </c>
       <c r="E17" s="23">
-        <f>IF(($R$3*$R$4)=1,1,-1)*(($M17/3.1416*180)+$N$5)</f>
+        <f>IF(($S$3*$S$4)=1,1,-1)*(($N17/3.1416*180)+$O$5)</f>
         <v>-30.000140305771573</v>
       </c>
       <c r="F17" s="11">
         <v>5</v>
       </c>
       <c r="G17" s="25">
-        <f t="shared" ref="G17" si="9">IF($R$3*$R$4=-1,1,0)</f>
+        <f t="shared" ref="G17" si="10">IF($S$3*$S$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
@@ -6512,18 +6713,22 @@
       <c r="L17" s="5">
         <v>13</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="69">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N17" s="6">
         <v>1.0471975511966001</v>
       </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="42">
+      <c r="O17" s="4"/>
+      <c r="P17" s="42">
         <v>100</v>
       </c>
-      <c r="P17" s="43">
+      <c r="Q17" s="43">
         <v>192.37604307033999</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="34"/>
       <c r="C18" s="23"/>
@@ -6541,18 +6746,22 @@
       <c r="L18" s="5">
         <v>20</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="68">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="N18" s="6">
         <v>2.0943951023932001</v>
       </c>
-      <c r="N18" s="4"/>
-      <c r="O18" s="42">
+      <c r="O18" s="4"/>
+      <c r="P18" s="42">
         <v>84</v>
       </c>
-      <c r="P18" s="43">
+      <c r="Q18" s="43">
         <v>183.138438763306</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -6570,18 +6779,22 @@
       <c r="L19" s="5">
         <v>32</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="68">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="N19" s="6">
         <v>2.0943951023932001</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="42">
+      <c r="O19" s="4"/>
+      <c r="P19" s="42">
         <v>100</v>
       </c>
-      <c r="P19" s="43">
+      <c r="Q19" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -6599,18 +6812,22 @@
       <c r="L20" s="5">
         <v>21</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="68">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="N20" s="6">
         <v>1.0471975511966001</v>
       </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="42">
+      <c r="O20" s="4"/>
+      <c r="P20" s="42">
         <v>84</v>
       </c>
-      <c r="P20" s="43">
+      <c r="Q20" s="43">
         <v>164.66323014923799</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
@@ -6628,18 +6845,22 @@
       <c r="L21" s="5">
         <v>43</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="68">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="N21" s="6">
         <v>2.0943951023932001</v>
       </c>
-      <c r="N21" s="4"/>
-      <c r="O21" s="42">
+      <c r="O21" s="4"/>
+      <c r="P21" s="42">
         <v>68</v>
       </c>
-      <c r="P21" s="43">
+      <c r="Q21" s="43">
         <v>155.425625842204</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -6657,18 +6878,22 @@
       <c r="L22" s="5">
         <v>10</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="68">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="6">
         <v>3.14159265358979</v>
       </c>
-      <c r="N22" s="4"/>
-      <c r="O22" s="42">
+      <c r="O22" s="4"/>
+      <c r="P22" s="42">
         <v>68</v>
       </c>
-      <c r="P22" s="43">
+      <c r="Q22" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -6686,18 +6911,22 @@
       <c r="L23" s="5">
         <v>33</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="68">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="N23" s="6">
         <v>3.14159265358979</v>
       </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="42">
+      <c r="O23" s="4"/>
+      <c r="P23" s="42">
         <v>100</v>
       </c>
-      <c r="P23" s="43">
+      <c r="Q23" s="43">
         <v>136.95041722813599</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="34"/>
       <c r="C24" s="23"/>
@@ -6715,18 +6944,22 @@
       <c r="L24" s="5">
         <v>42</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M24" s="68">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="N24" s="6">
         <v>2.0943951023932001</v>
       </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="42">
+      <c r="O24" s="4"/>
+      <c r="P24" s="42">
         <v>84</v>
       </c>
-      <c r="P24" s="43">
+      <c r="Q24" s="43">
         <v>127.712812921102</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -6744,25 +6977,105 @@
       <c r="L25" s="46">
         <v>43</v>
       </c>
-      <c r="M25" s="47">
+      <c r="M25" s="68">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="N25" s="47">
         <v>3.14159265358979</v>
       </c>
-      <c r="N25" s="48"/>
-      <c r="O25" s="49">
+      <c r="O25" s="48"/>
+      <c r="P25" s="49">
         <v>84</v>
       </c>
-      <c r="P25" s="50">
+      <c r="Q25" s="50">
         <v>109.237604307034</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M31" s="7"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="8"/>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M35" s="8"/>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M37" s="8"/>
+    </row>
+    <row r="38" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M38" s="8"/>
+    </row>
+    <row r="39" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M39" s="8"/>
+    </row>
+    <row r="40" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M40" s="8"/>
+    </row>
+    <row r="41" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M41" s="8"/>
+    </row>
+    <row r="42" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M42" s="8"/>
+    </row>
+    <row r="43" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M43" s="8"/>
+    </row>
+    <row r="44" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M44" s="8"/>
+    </row>
+    <row r="45" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M45" s="8"/>
+    </row>
+    <row r="46" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M46" s="8"/>
+    </row>
+    <row r="47" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M47" s="8"/>
+    </row>
+    <row r="48" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M48" s="8"/>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M49" s="8"/>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M50" s="8"/>
+    </row>
+    <row r="51" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M51" s="8"/>
+    </row>
+    <row r="52" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M52" s="8"/>
+    </row>
+    <row r="53" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M53" s="8"/>
+    </row>
+    <row r="54" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M54" s="8"/>
+    </row>
+    <row r="55" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M55" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6770,7 +7083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G48" sqref="A3:G48"/>
     </sheetView>
   </sheetViews>

</xml_diff>